<commit_message>
Update spreadsheets to include equipment calibration dates
</commit_message>
<xml_diff>
--- a/MUSCBoneDensity.xlsx
+++ b/MUSCBoneDensity.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="113">
   <si>
     <t>Print Area</t>
   </si>
@@ -341,9 +341,6 @@
     <t>Piranha CB2-17090320</t>
   </si>
   <si>
-    <t>Piranha R100B</t>
-  </si>
-  <si>
     <t>Detector entrance dose measurements</t>
   </si>
   <si>
@@ -357,6 +354,18 @@
   </si>
   <si>
     <t>Revision 1.3-20190605</t>
+  </si>
+  <si>
+    <t>Calibration date:</t>
+  </si>
+  <si>
+    <t>Calibration due:</t>
+  </si>
+  <si>
+    <t>Test equipment:</t>
+  </si>
+  <si>
+    <t>R100B</t>
   </si>
 </sst>
 </file>
@@ -367,9 +376,9 @@
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="dd\-mmm\-yy"/>
     <numFmt numFmtId="166" formatCode="mmm\-yyyy"/>
-    <numFmt numFmtId="168" formatCode="0.0"/>
-    <numFmt numFmtId="169" formatCode="0.000"/>
-    <numFmt numFmtId="171" formatCode="[$-409]d/mmm/yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="169" formatCode="[$-409]d/mmm/yyyy;@"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -469,7 +478,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -924,6 +933,30 @@
         <color auto="1"/>
       </left>
       <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="double">
         <color auto="1"/>
       </right>
       <top/>
@@ -944,7 +977,7 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1175,7 +1208,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1184,7 +1217,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="168" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1205,6 +1238,34 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="4" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1229,31 +1290,42 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="4" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="171" fontId="4" fillId="3" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="171" fontId="4" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="171" fontId="4" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="169" fontId="4" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="10" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading" xfId="3"/>
@@ -1262,7 +1334,7 @@
     <cellStyle name="Result" xfId="1"/>
     <cellStyle name="Result2" xfId="2"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1270,16 +1342,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1669,7 +1731,7 @@
       <c r="L1" s="7"/>
       <c r="M1" s="8"/>
       <c r="O1" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="P1" s="10"/>
       <c r="Q1" s="10"/>
@@ -1836,7 +1898,7 @@
       <c r="O7" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="P7" s="134"/>
+      <c r="P7" s="120"/>
       <c r="Q7" s="31"/>
       <c r="R7" s="13"/>
       <c r="S7" s="13"/>
@@ -1876,7 +1938,7 @@
       <c r="O8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="P8" s="135" t="str">
+      <c r="P8" s="121" t="str">
         <f>IF(AB8="","",AB8)</f>
         <v/>
       </c>
@@ -1894,12 +1956,12 @@
       <c r="AA8" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="AB8" s="137"/>
+      <c r="AB8" s="123"/>
       <c r="AC8" s="35" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="AD8" s="138" t="str">
+      <c r="AD8" s="124" t="str">
         <f>IF(P7="","",P7)</f>
         <v/>
       </c>
@@ -1961,19 +2023,19 @@
       <c r="E10" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="128" t="str">
+      <c r="F10" s="125" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="128"/>
+      <c r="G10" s="125"/>
       <c r="J10" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="128" t="str">
+      <c r="K10" s="125" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="128"/>
+      <c r="L10" s="125"/>
       <c r="M10" s="15"/>
       <c r="O10" s="55"/>
       <c r="P10" s="13"/>
@@ -2017,19 +2079,19 @@
       <c r="E11" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="131" t="str">
+      <c r="F11" s="126" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="131"/>
+      <c r="G11" s="126"/>
       <c r="J11" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="131" t="str">
+      <c r="K11" s="126" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="131"/>
+      <c r="L11" s="126"/>
       <c r="M11" s="15"/>
       <c r="O11" s="55"/>
       <c r="P11" s="13"/>
@@ -2073,19 +2135,19 @@
       <c r="E12" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="131" t="str">
+      <c r="F12" s="126" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="131"/>
+      <c r="G12" s="126"/>
       <c r="J12" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="133" t="str">
+      <c r="K12" s="127" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="133"/>
+      <c r="L12" s="127"/>
       <c r="M12" s="15"/>
       <c r="O12" s="55"/>
       <c r="P12" s="13"/>
@@ -2129,14 +2191,14 @@
       <c r="E13" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="131" t="str">
+      <c r="F13" s="126" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="131"/>
+      <c r="G13" s="126"/>
       <c r="J13" s="52"/>
-      <c r="K13" s="132"/>
-      <c r="L13" s="132"/>
+      <c r="K13" s="128"/>
+      <c r="L13" s="128"/>
       <c r="M13" s="15"/>
       <c r="O13" s="55"/>
       <c r="P13" s="13"/>
@@ -2237,19 +2299,19 @@
       <c r="E16" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="128" t="str">
+      <c r="F16" s="125" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="128"/>
+      <c r="G16" s="125"/>
       <c r="J16" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="K16" s="130" t="str">
+      <c r="K16" s="129" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="130"/>
+      <c r="L16" s="129"/>
       <c r="M16" s="15"/>
       <c r="O16" s="55"/>
       <c r="P16" s="62" t="s">
@@ -2285,19 +2347,19 @@
       <c r="E17" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="128" t="str">
+      <c r="F17" s="125" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="128"/>
+      <c r="G17" s="125"/>
       <c r="J17" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="K17" s="128" t="str">
+      <c r="K17" s="125" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="128"/>
+      <c r="L17" s="125"/>
       <c r="M17" s="15"/>
       <c r="O17" s="55"/>
       <c r="P17" s="13"/>
@@ -2341,19 +2403,19 @@
       <c r="E18" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="128" t="str">
+      <c r="F18" s="125" t="str">
         <f>IF(R19="","",R19)</f>
         <v/>
       </c>
-      <c r="G18" s="128"/>
+      <c r="G18" s="125"/>
       <c r="J18" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="128" t="str">
+      <c r="K18" s="125" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="128"/>
+      <c r="L18" s="125"/>
       <c r="M18" s="15"/>
       <c r="O18" s="55"/>
       <c r="P18" s="13"/>
@@ -2442,19 +2504,19 @@
       <c r="E21" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="128" t="str">
+      <c r="F21" s="125" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="128"/>
+      <c r="G21" s="125"/>
       <c r="J21" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="K21" s="128" t="str">
+      <c r="K21" s="125" t="str">
         <f>IF(V22="","",V22)</f>
         <v/>
       </c>
-      <c r="L21" s="128"/>
+      <c r="L21" s="125"/>
       <c r="M21" s="15"/>
       <c r="O21" s="55"/>
       <c r="P21" s="62" t="s">
@@ -2492,19 +2554,19 @@
       <c r="E22" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="130" t="str">
+      <c r="F22" s="129" t="str">
         <f>IF(R23="","",R23)</f>
         <v/>
       </c>
-      <c r="G22" s="130"/>
+      <c r="G22" s="129"/>
       <c r="J22" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="K22" s="128" t="str">
+      <c r="K22" s="125" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="128"/>
+      <c r="L22" s="125"/>
       <c r="M22" s="15"/>
       <c r="O22" s="55"/>
       <c r="P22" s="13"/>
@@ -2551,11 +2613,11 @@
       <c r="J23" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="K23" s="128" t="str">
+      <c r="K23" s="125" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="128"/>
+      <c r="L23" s="125"/>
       <c r="M23" s="15"/>
       <c r="O23" s="55"/>
       <c r="P23" s="13"/>
@@ -2599,11 +2661,11 @@
       <c r="E24" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="128" t="str">
+      <c r="F24" s="125" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="128"/>
+      <c r="G24" s="125"/>
       <c r="M24" s="15"/>
       <c r="O24" s="55"/>
       <c r="P24" s="62" t="s">
@@ -2644,11 +2706,11 @@
       <c r="E25" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="128" t="str">
+      <c r="F25" s="125" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="128"/>
+      <c r="G25" s="125"/>
       <c r="J25" s="61" t="s">
         <v>39</v>
       </c>
@@ -2690,19 +2752,19 @@
       <c r="E26" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="128" t="str">
+      <c r="F26" s="125" t="str">
         <f>IF(R27="","",R27)</f>
         <v/>
       </c>
-      <c r="G26" s="128"/>
+      <c r="G26" s="125"/>
       <c r="J26" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="K26" s="128" t="str">
+      <c r="K26" s="125" t="str">
         <f>IF(V27="","",V27)</f>
         <v/>
       </c>
-      <c r="L26" s="128"/>
+      <c r="L26" s="125"/>
       <c r="M26" s="15"/>
       <c r="O26" s="55"/>
       <c r="P26" s="13"/>
@@ -2746,11 +2808,11 @@
       <c r="J27" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="K27" s="128" t="str">
+      <c r="K27" s="125" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="128"/>
+      <c r="L27" s="125"/>
       <c r="M27" s="15"/>
       <c r="O27" s="55"/>
       <c r="P27" s="13"/>
@@ -2787,11 +2849,11 @@
       <c r="E28" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="128" t="str">
+      <c r="F28" s="125" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="128"/>
+      <c r="G28" s="125"/>
       <c r="M28" s="15"/>
       <c r="O28" s="55"/>
       <c r="P28" s="62" t="s">
@@ -2832,11 +2894,11 @@
       <c r="E29" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="128" t="str">
+      <c r="F29" s="125" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="128"/>
+      <c r="G29" s="125"/>
       <c r="M29" s="15"/>
       <c r="O29" s="55"/>
       <c r="P29" s="13"/>
@@ -2875,11 +2937,11 @@
       <c r="E30" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F30" s="128" t="str">
+      <c r="F30" s="125" t="str">
         <f>IF(R31="","",R31)</f>
         <v/>
       </c>
-      <c r="G30" s="128"/>
+      <c r="G30" s="125"/>
       <c r="M30" s="15"/>
       <c r="O30" s="55"/>
       <c r="P30" s="13"/>
@@ -3023,10 +3085,10 @@
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
-      <c r="L34" s="129" t="s">
+      <c r="L34" s="130" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="129"/>
+      <c r="M34" s="130"/>
       <c r="O34" s="13"/>
       <c r="P34" s="13"/>
       <c r="Q34" s="13"/>
@@ -3314,7 +3376,7 @@
         <v>Change</v>
       </c>
       <c r="AD42" s="50" t="str">
-        <f>IF(U92="","",U92)</f>
+        <f>IF(U94="","",U94)</f>
         <v>Piranha CB2-17090320</v>
       </c>
     </row>
@@ -3348,8 +3410,8 @@
         <v>Change</v>
       </c>
       <c r="AD43" s="50" t="str">
-        <f>IF(X93="","",X93)</f>
-        <v>Piranha R100B</v>
+        <f>IF(X95="","",X95)</f>
+        <v>R100B</v>
       </c>
     </row>
     <row r="44" spans="1:30" ht="15.75" customHeight="1">
@@ -3550,10 +3612,10 @@
         <v>55</v>
       </c>
       <c r="O55" s="75"/>
-      <c r="S55" s="119" t="s">
+      <c r="S55" s="131" t="s">
         <v>68</v>
       </c>
-      <c r="T55" s="119"/>
+      <c r="T55" s="131"/>
       <c r="Y55" s="76"/>
     </row>
     <row r="56" spans="1:25" ht="15.75" customHeight="1">
@@ -3651,7 +3713,7 @@
       <c r="C59" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D59" s="136" t="str">
+      <c r="D59" s="122" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -3801,10 +3863,10 @@
         <v>4</v>
       </c>
       <c r="B64" s="14"/>
-      <c r="H64" s="120" t="s">
+      <c r="H64" s="132" t="s">
         <v>93</v>
       </c>
-      <c r="I64" s="121"/>
+      <c r="I64" s="133"/>
       <c r="K64" s="61" t="s">
         <v>67</v>
       </c>
@@ -3898,11 +3960,11 @@
       <c r="Q66" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="R66" s="119" t="s">
+      <c r="R66" s="131" t="s">
         <v>91</v>
       </c>
-      <c r="S66" s="119"/>
-      <c r="T66" s="119"/>
+      <c r="S66" s="131"/>
+      <c r="T66" s="131"/>
       <c r="U66" s="4" t="s">
         <v>91</v>
       </c>
@@ -4144,11 +4206,11 @@
       <c r="Q72" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="R72" s="119" t="s">
+      <c r="R72" s="131" t="s">
         <v>91</v>
       </c>
-      <c r="S72" s="119"/>
-      <c r="T72" s="119"/>
+      <c r="S72" s="131"/>
+      <c r="T72" s="131"/>
       <c r="U72" s="4" t="s">
         <v>91</v>
       </c>
@@ -4314,16 +4376,16 @@
       <c r="G77" s="97" t="s">
         <v>92</v>
       </c>
-      <c r="I77" s="124" t="s">
+      <c r="I77" s="136" t="s">
         <v>69</v>
       </c>
-      <c r="J77" s="126" t="s">
+      <c r="J77" s="138" t="s">
         <v>95</v>
       </c>
-      <c r="K77" s="122" t="s">
+      <c r="K77" s="134" t="s">
         <v>96</v>
       </c>
-      <c r="L77" s="123"/>
+      <c r="L77" s="135"/>
       <c r="M77" s="15"/>
       <c r="O77" s="75"/>
       <c r="Y77" s="76"/>
@@ -4349,8 +4411,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I78" s="125"/>
-      <c r="J78" s="127"/>
+      <c r="I78" s="137"/>
+      <c r="J78" s="139"/>
       <c r="K78" s="97" t="s">
         <v>97</v>
       </c>
@@ -4368,11 +4430,11 @@
       <c r="Q78" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="R78" s="119" t="s">
+      <c r="R78" s="131" t="s">
         <v>91</v>
       </c>
-      <c r="S78" s="119"/>
-      <c r="T78" s="119"/>
+      <c r="S78" s="131"/>
+      <c r="T78" s="131"/>
       <c r="U78" s="4" t="s">
         <v>91</v>
       </c>
@@ -4403,19 +4465,19 @@
         <v/>
       </c>
       <c r="I79" s="97" t="str">
-        <f>IF(O98="","",O98)</f>
+        <f>IF(O100="","",O100)</f>
         <v>High Def</v>
       </c>
       <c r="J79" s="114" t="str">
-        <f>IF(S98="","",S98)</f>
+        <f>IF(S100="","",S100)</f>
         <v/>
       </c>
       <c r="K79" s="114" t="str">
-        <f t="shared" ref="K79:L82" si="7">IF(U98="","",U98)</f>
+        <f>IF(U100="","",U100)</f>
         <v/>
       </c>
       <c r="L79" s="114" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(V100="","",V100)</f>
         <v/>
       </c>
       <c r="M79" s="15"/>
@@ -4463,19 +4525,19 @@
         <v/>
       </c>
       <c r="I80" s="97" t="str">
-        <f>IF(O99="","",O99)</f>
+        <f>IF(O101="","",O101)</f>
         <v>Array</v>
       </c>
       <c r="J80" s="114" t="str">
-        <f>IF(S99="","",S99)</f>
+        <f>IF(S101="","",S101)</f>
         <v/>
       </c>
       <c r="K80" s="114" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(U101="","",U101)</f>
         <v/>
       </c>
       <c r="L80" s="114" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(V101="","",V101)</f>
         <v/>
       </c>
       <c r="M80" s="15"/>
@@ -4523,19 +4585,19 @@
         <v/>
       </c>
       <c r="I81" s="97" t="str">
-        <f>IF(O100="","",O100)</f>
+        <f>IF(O102="","",O102)</f>
         <v>Fast Array</v>
       </c>
       <c r="J81" s="114" t="str">
-        <f>IF(S100="","",S100)</f>
+        <f>IF(S102="","",S102)</f>
         <v/>
       </c>
       <c r="K81" s="114" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(U102="","",U102)</f>
         <v/>
       </c>
       <c r="L81" s="114" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(V102="","",V102)</f>
         <v/>
       </c>
       <c r="M81" s="15"/>
@@ -4567,19 +4629,19 @@
       </c>
       <c r="B82" s="14"/>
       <c r="I82" s="97" t="str">
-        <f>IF(O101="","",O101)</f>
+        <f>IF(O103="","",O103)</f>
         <v>Turbo</v>
       </c>
       <c r="J82" s="114" t="str">
-        <f>IF(S101="","",S101)</f>
+        <f>IF(S103="","",S103)</f>
         <v/>
       </c>
       <c r="K82" s="114" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(U103="","",U103)</f>
         <v/>
       </c>
       <c r="L82" s="114" t="str">
-        <f t="shared" si="7"/>
+        <f>IF(V103="","",V103)</f>
         <v/>
       </c>
       <c r="M82" s="15"/>
@@ -4636,22 +4698,35 @@
       </c>
       <c r="B84" s="14"/>
       <c r="D84" s="97" t="str">
-        <f t="shared" ref="D84:E87" si="8">IF(P73="","",P73)</f>
+        <f t="shared" ref="D84:E87" si="7">IF(P73="","",P73)</f>
         <v>Tableside</v>
       </c>
       <c r="E84" s="118" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="F84" s="113" t="str">
+        <f t="shared" ref="F84:G87" si="8">IF(U73="","",U73)</f>
+        <v/>
+      </c>
+      <c r="G84" s="114" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="F84" s="113" t="str">
-        <f t="shared" ref="F84:G87" si="9">IF(U73="","",U73)</f>
-        <v/>
-      </c>
-      <c r="G84" s="114" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="M84" s="15"/>
+      <c r="I84" s="145" t="s">
+        <v>111</v>
+      </c>
+      <c r="J84" s="146" t="str">
+        <f>IF(U94="","",U94)</f>
+        <v>Piranha CB2-17090320</v>
+      </c>
+      <c r="L84" s="151" t="s">
+        <v>60</v>
+      </c>
+      <c r="M84" s="153" t="str">
+        <f>IF(X94="","",X94)</f>
+        <v>R100B</v>
+      </c>
       <c r="O84" s="93" t="str">
         <f>IF(O60="","",O60)</f>
         <v>Turbo</v>
@@ -4662,11 +4737,11 @@
       <c r="Q84" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="R84" s="119" t="s">
+      <c r="R84" s="131" t="s">
         <v>91</v>
       </c>
-      <c r="S84" s="119"/>
-      <c r="T84" s="119"/>
+      <c r="S84" s="131"/>
+      <c r="T84" s="131"/>
       <c r="U84" s="4" t="s">
         <v>91</v>
       </c>
@@ -4681,22 +4756,32 @@
       </c>
       <c r="B85" s="14"/>
       <c r="D85" s="97" t="str">
+        <f t="shared" si="7"/>
+        <v>Operator</v>
+      </c>
+      <c r="E85" s="118" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="F85" s="113" t="str">
         <f t="shared" si="8"/>
-        <v>Operator</v>
-      </c>
-      <c r="E85" s="118" t="str">
+        <v/>
+      </c>
+      <c r="G85" s="114" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="F85" s="113" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="G85" s="114" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="M85" s="15"/>
+      <c r="I85" s="145" t="s">
+        <v>109</v>
+      </c>
+      <c r="J85" s="147"/>
+      <c r="L85" s="151" t="s">
+        <v>109</v>
+      </c>
+      <c r="M85" s="152" t="str">
+        <f>IF(X96="","",X96)</f>
+        <v/>
+      </c>
       <c r="O85" s="75"/>
       <c r="P85" s="92" t="str">
         <f>IF($V$57="","",$V$57)</f>
@@ -4725,22 +4810,35 @@
       </c>
       <c r="B86" s="14"/>
       <c r="D86" s="97" t="str">
+        <f t="shared" si="7"/>
+        <v>Door</v>
+      </c>
+      <c r="E86" s="118" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="F86" s="113" t="str">
         <f t="shared" si="8"/>
-        <v>Door</v>
-      </c>
-      <c r="E86" s="118" t="str">
+        <v/>
+      </c>
+      <c r="G86" s="114" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="F86" s="113" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="G86" s="114" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="M86" s="15"/>
+      <c r="I86" s="145" t="s">
+        <v>110</v>
+      </c>
+      <c r="J86" s="148" t="str">
+        <f>IF(U96="","",U96)</f>
+        <v/>
+      </c>
+      <c r="L86" s="151" t="s">
+        <v>110</v>
+      </c>
+      <c r="M86" s="152" t="str">
+        <f>IF(X97="","",X97)</f>
+        <v/>
+      </c>
       <c r="O86" s="75"/>
       <c r="P86" s="92" t="str">
         <f>IF($V$58="","",$V$58)</f>
@@ -4769,19 +4867,19 @@
       </c>
       <c r="B87" s="14"/>
       <c r="D87" s="97" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="E87" s="118" t="str">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+      <c r="F87" s="113" t="str">
         <f t="shared" si="8"/>
         <v/>
       </c>
-      <c r="E87" s="118" t="str">
+      <c r="G87" s="114" t="str">
         <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="F87" s="113" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-      <c r="G87" s="114" t="str">
-        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M87" s="15"/>
@@ -4835,7 +4933,7 @@
       </c>
       <c r="Y88" s="76"/>
     </row>
-    <row r="89" spans="1:25" ht="15.75" customHeight="1" thickBot="1">
+    <row r="89" spans="1:25" ht="15.75" customHeight="1">
       <c r="A89" s="5">
         <v>29</v>
       </c>
@@ -4857,17 +4955,8 @@
         <v>92</v>
       </c>
       <c r="M89" s="15"/>
-      <c r="O89" s="80"/>
-      <c r="P89" s="81"/>
-      <c r="Q89" s="81"/>
-      <c r="R89" s="81"/>
-      <c r="S89" s="81"/>
-      <c r="T89" s="81"/>
-      <c r="U89" s="81"/>
-      <c r="V89" s="81"/>
-      <c r="W89" s="81"/>
-      <c r="X89" s="81"/>
-      <c r="Y89" s="82"/>
+      <c r="O89" s="75"/>
+      <c r="Y89" s="76"/>
     </row>
     <row r="90" spans="1:25" ht="15.75" customHeight="1">
       <c r="A90" s="5">
@@ -4875,60 +4964,70 @@
       </c>
       <c r="B90" s="14"/>
       <c r="D90" s="97" t="str">
-        <f t="shared" ref="D90:E93" si="10">IF(P79="","",P79)</f>
+        <f t="shared" ref="D90:E93" si="9">IF(P79="","",P79)</f>
         <v>Tableside</v>
       </c>
       <c r="E90" s="118" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F90" s="113" t="str">
+        <f t="shared" ref="F90:G93" si="10">IF(U79="","",U79)</f>
+        <v/>
+      </c>
+      <c r="G90" s="114" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="F90" s="113" t="str">
-        <f t="shared" ref="F90:G93" si="11">IF(U79="","",U79)</f>
-        <v/>
-      </c>
-      <c r="G90" s="114" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
       <c r="M90" s="15"/>
-      <c r="O90" s="105"/>
-      <c r="P90" s="84"/>
-      <c r="Q90" s="84"/>
-      <c r="R90" s="84"/>
-      <c r="S90" s="84"/>
-      <c r="T90" s="84"/>
-      <c r="U90" s="84"/>
-      <c r="V90" s="84"/>
-      <c r="W90" s="84"/>
-      <c r="X90" s="84"/>
-      <c r="Y90" s="86"/>
-    </row>
-    <row r="91" spans="1:25" ht="15.75" customHeight="1">
+      <c r="O90" s="75"/>
+      <c r="P90" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q90" s="140"/>
+      <c r="S90" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="T90" s="142"/>
+      <c r="V90" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="W90" s="142"/>
+      <c r="Y90" s="76"/>
+    </row>
+    <row r="91" spans="1:25" ht="15.75" customHeight="1" thickBot="1">
       <c r="A91" s="5">
         <v>31</v>
       </c>
       <c r="B91" s="14"/>
       <c r="D91" s="97" t="str">
+        <f t="shared" si="9"/>
+        <v>Operator</v>
+      </c>
+      <c r="E91" s="118" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F91" s="113" t="str">
         <f t="shared" si="10"/>
-        <v>Operator</v>
-      </c>
-      <c r="E91" s="118" t="str">
+        <v/>
+      </c>
+      <c r="G91" s="114" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="F91" s="113" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="G91" s="114" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
       <c r="M91" s="15"/>
-      <c r="O91" s="90" t="s">
-        <v>99</v>
-      </c>
-      <c r="Y91" s="76"/>
+      <c r="O91" s="80"/>
+      <c r="P91" s="81"/>
+      <c r="Q91" s="81"/>
+      <c r="R91" s="81"/>
+      <c r="S91" s="81"/>
+      <c r="T91" s="81"/>
+      <c r="U91" s="81"/>
+      <c r="V91" s="81"/>
+      <c r="W91" s="81"/>
+      <c r="X91" s="81"/>
+      <c r="Y91" s="82"/>
     </row>
     <row r="92" spans="1:25" ht="15.75" customHeight="1">
       <c r="A92" s="5">
@@ -4936,44 +5035,33 @@
       </c>
       <c r="B92" s="14"/>
       <c r="D92" s="97" t="str">
+        <f t="shared" si="9"/>
+        <v>Door</v>
+      </c>
+      <c r="E92" s="118" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F92" s="113" t="str">
         <f t="shared" si="10"/>
-        <v>Door</v>
-      </c>
-      <c r="E92" s="118" t="str">
+        <v/>
+      </c>
+      <c r="G92" s="114" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="F92" s="113" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="G92" s="114" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
       <c r="M92" s="15"/>
-      <c r="O92" s="77">
-        <v>107</v>
-      </c>
-      <c r="P92" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="T92" s="22" t="s">
-        <v>101</v>
-      </c>
-      <c r="U92" s="32" t="str">
-        <f>IF(U93&lt;&gt;"",U93,IF(AB42="","",AB42))</f>
-        <v>Piranha CB2-17090320</v>
-      </c>
-      <c r="V92" s="32"/>
-      <c r="W92" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="X92" s="32" t="str">
-        <f>IF(X93&lt;&gt;"",X93,IF(AB43="","",AB43))</f>
-        <v>Piranha R100B</v>
-      </c>
-      <c r="Y92" s="76"/>
+      <c r="O92" s="105"/>
+      <c r="P92" s="84"/>
+      <c r="Q92" s="84"/>
+      <c r="R92" s="84"/>
+      <c r="S92" s="84"/>
+      <c r="T92" s="84"/>
+      <c r="U92" s="84"/>
+      <c r="V92" s="84"/>
+      <c r="W92" s="84"/>
+      <c r="X92" s="84"/>
+      <c r="Y92" s="86"/>
     </row>
     <row r="93" spans="1:25" ht="15.75" customHeight="1">
       <c r="A93" s="5">
@@ -4981,34 +5069,24 @@
       </c>
       <c r="B93" s="14"/>
       <c r="D93" s="97" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="E93" s="118" t="str">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="F93" s="113" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="E93" s="118" t="str">
+      <c r="G93" s="114" t="str">
         <f t="shared" si="10"/>
         <v/>
       </c>
-      <c r="F93" s="113" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-      <c r="G93" s="114" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
       <c r="M93" s="15"/>
-      <c r="O93" s="77">
-        <v>42.4</v>
-      </c>
-      <c r="P93" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="U93" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="V93" s="33"/>
-      <c r="X93" s="33" t="s">
-        <v>104</v>
+      <c r="O93" s="90" t="s">
+        <v>99</v>
       </c>
       <c r="Y93" s="76"/>
     </row>
@@ -5018,9 +5096,27 @@
       </c>
       <c r="B94" s="14"/>
       <c r="M94" s="15"/>
-      <c r="O94" s="75"/>
-      <c r="T94" s="106"/>
-      <c r="U94" s="106"/>
+      <c r="O94" s="77">
+        <v>107</v>
+      </c>
+      <c r="P94" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="T94" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="U94" s="143" t="str">
+        <f>IF(U95&lt;&gt;"",U95,IF(AB42="","",AB42))</f>
+        <v>Piranha CB2-17090320</v>
+      </c>
+      <c r="V94" s="143"/>
+      <c r="W94" s="22" t="s">
+        <v>60</v>
+      </c>
+      <c r="X94" s="141" t="str">
+        <f>IF(X95&lt;&gt;"",X95,IF(AB43="","",AB43))</f>
+        <v>R100B</v>
+      </c>
       <c r="Y94" s="76"/>
     </row>
     <row r="95" spans="1:25" ht="15.75" customHeight="1">
@@ -5045,11 +5141,19 @@
         <v>92</v>
       </c>
       <c r="M95" s="15"/>
-      <c r="O95" s="90" t="s">
-        <v>105</v>
-      </c>
-      <c r="T95" s="106"/>
-      <c r="U95" s="106"/>
+      <c r="O95" s="77">
+        <v>42.4</v>
+      </c>
+      <c r="P95" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="U95" s="144" t="s">
+        <v>103</v>
+      </c>
+      <c r="V95" s="144"/>
+      <c r="X95" s="140" t="s">
+        <v>112</v>
+      </c>
       <c r="Y95" s="76"/>
     </row>
     <row r="96" spans="1:25" ht="15.75" customHeight="1">
@@ -5058,34 +5162,31 @@
       </c>
       <c r="B96" s="14"/>
       <c r="D96" s="97" t="str">
-        <f t="shared" ref="D96:E99" si="12">IF(P85="","",P85)</f>
+        <f t="shared" ref="D96:E99" si="11">IF(P85="","",P85)</f>
         <v>Tableside</v>
       </c>
       <c r="E96" s="118" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="F96" s="113" t="str">
+        <f t="shared" ref="F96:G99" si="12">IF(U85="","",U85)</f>
+        <v/>
+      </c>
+      <c r="G96" s="114" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="F96" s="113" t="str">
-        <f t="shared" ref="F96:G99" si="13">IF(U85="","",U85)</f>
-        <v/>
-      </c>
-      <c r="G96" s="114" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
       <c r="M96" s="15"/>
-      <c r="O96" s="107"/>
-      <c r="P96" s="106"/>
-      <c r="Q96" s="106"/>
-      <c r="R96" s="106"/>
-      <c r="S96" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="T96" s="106"/>
-      <c r="U96" s="119" t="s">
-        <v>106</v>
-      </c>
-      <c r="V96" s="119"/>
+      <c r="O96" s="75"/>
+      <c r="T96" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="U96" s="142"/>
+      <c r="W96" s="22" t="s">
+        <v>109</v>
+      </c>
+      <c r="X96" s="142"/>
       <c r="Y96" s="76"/>
     </row>
     <row r="97" spans="1:25" ht="15.75" customHeight="1">
@@ -5094,42 +5195,33 @@
       </c>
       <c r="B97" s="14"/>
       <c r="D97" s="97" t="str">
+        <f t="shared" si="11"/>
+        <v>Operator</v>
+      </c>
+      <c r="E97" s="118" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="F97" s="113" t="str">
         <f t="shared" si="12"/>
-        <v>Operator</v>
-      </c>
-      <c r="E97" s="118" t="str">
+        <v/>
+      </c>
+      <c r="G97" s="114" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="F97" s="113" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="G97" s="114" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
       <c r="M97" s="15"/>
-      <c r="O97" s="108" t="s">
-        <v>69</v>
-      </c>
-      <c r="P97" s="119" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q97" s="119"/>
-      <c r="R97" s="119"/>
-      <c r="S97" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="T97" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="U97" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="V97" s="4" t="s">
-        <v>98</v>
-      </c>
+      <c r="O97" s="90" t="s">
+        <v>104</v>
+      </c>
+      <c r="T97" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="U97" s="142"/>
+      <c r="W97" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="X97" s="142"/>
       <c r="Y97" s="76"/>
     </row>
     <row r="98" spans="1:25" ht="15.75" customHeight="1">
@@ -5138,45 +5230,34 @@
       </c>
       <c r="B98" s="14"/>
       <c r="D98" s="97" t="str">
+        <f t="shared" si="11"/>
+        <v>Door</v>
+      </c>
+      <c r="E98" s="118" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="F98" s="113" t="str">
         <f t="shared" si="12"/>
-        <v>Door</v>
-      </c>
-      <c r="E98" s="118" t="str">
+        <v/>
+      </c>
+      <c r="G98" s="114" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="F98" s="113" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="G98" s="114" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
       <c r="M98" s="15"/>
-      <c r="O98" s="109" t="str">
-        <f>IF(O57="","",O57)</f>
-        <v>High Def</v>
-      </c>
-      <c r="P98" s="89"/>
-      <c r="Q98" s="89"/>
-      <c r="R98" s="89"/>
-      <c r="S98" s="110" t="str">
-        <f>IF(P98="","",AVERAGE(P98:R98))</f>
-        <v/>
-      </c>
-      <c r="T98" s="110" t="str">
-        <f>IF(P98="","",STDEV(P98:R98))</f>
-        <v/>
-      </c>
-      <c r="U98" s="95" t="str">
-        <f>IF(S98="","",S98*($O$92/$O$93)^2)</f>
-        <v/>
-      </c>
-      <c r="V98" s="95" t="str">
-        <f>IF(U98="","",U98/R57)</f>
-        <v/>
-      </c>
+      <c r="O98" s="107"/>
+      <c r="P98" s="106"/>
+      <c r="Q98" s="106"/>
+      <c r="R98" s="106"/>
+      <c r="S98" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="T98" s="106"/>
+      <c r="U98" s="119" t="s">
+        <v>105</v>
+      </c>
+      <c r="V98" s="119"/>
       <c r="Y98" s="76"/>
     </row>
     <row r="99" spans="1:25" ht="15.75" customHeight="1">
@@ -5185,66 +5266,53 @@
       </c>
       <c r="B99" s="14"/>
       <c r="D99" s="97" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="E99" s="118" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+      <c r="F99" s="113" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="E99" s="118" t="str">
+      <c r="G99" s="114" t="str">
         <f t="shared" si="12"/>
         <v/>
       </c>
-      <c r="F99" s="113" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
-      <c r="G99" s="114" t="str">
-        <f t="shared" si="13"/>
-        <v/>
-      </c>
       <c r="M99" s="15"/>
-      <c r="O99" s="109" t="str">
-        <f>IF(O58="","",O58)</f>
-        <v>Array</v>
-      </c>
-      <c r="P99" s="89"/>
-      <c r="Q99" s="89"/>
-      <c r="R99" s="89"/>
-      <c r="S99" s="110" t="str">
-        <f>IF(P99="","",AVERAGE(P99:R99))</f>
-        <v/>
-      </c>
-      <c r="T99" s="110" t="str">
-        <f>IF(P99="","",STDEV(P99:R99))</f>
-        <v/>
-      </c>
-      <c r="U99" s="95" t="str">
-        <f>IF(S99="","",S99*($O$92/$O$93)^2)</f>
-        <v/>
-      </c>
-      <c r="V99" s="95" t="str">
-        <f>IF(U99="","",U99/R58)</f>
-        <v/>
+      <c r="O99" s="108" t="s">
+        <v>69</v>
+      </c>
+      <c r="P99" s="119" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q99" s="119"/>
+      <c r="R99" s="119"/>
+      <c r="S99" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="T99" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="U99" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="V99" s="4" t="s">
+        <v>98</v>
       </c>
       <c r="Y99" s="76"/>
     </row>
-    <row r="100" spans="1:25" ht="15.75" customHeight="1" thickBot="1">
+    <row r="100" spans="1:25" ht="15.75" customHeight="1">
       <c r="A100" s="5">
         <v>40</v>
       </c>
-      <c r="B100" s="24"/>
-      <c r="C100" s="25"/>
-      <c r="D100" s="25"/>
-      <c r="E100" s="25"/>
-      <c r="F100" s="25"/>
-      <c r="G100" s="25"/>
-      <c r="H100" s="25"/>
-      <c r="I100" s="25"/>
-      <c r="J100" s="25"/>
-      <c r="K100" s="25"/>
-      <c r="L100" s="25"/>
-      <c r="M100" s="26"/>
+      <c r="B100" s="14"/>
+      <c r="M100" s="15"/>
       <c r="O100" s="109" t="str">
-        <f>IF(O59="","",O59)</f>
-        <v>Fast Array</v>
+        <f>IF(O57="","",O57)</f>
+        <v>High Def</v>
       </c>
       <c r="P100" s="89"/>
       <c r="Q100" s="89"/>
@@ -5258,22 +5326,31 @@
         <v/>
       </c>
       <c r="U100" s="95" t="str">
-        <f>IF(S100="","",S100*($O$92/$O$93)^2)</f>
+        <f>IF(S100="","",S100*($O$94/$O$95)^2)</f>
         <v/>
       </c>
       <c r="V100" s="95" t="str">
-        <f>IF(U100="","",U100/R59)</f>
+        <f>IF(U100="","",U100/R57)</f>
         <v/>
       </c>
       <c r="Y100" s="76"/>
     </row>
-    <row r="101" spans="1:25" ht="15.75" customHeight="1" thickTop="1">
+    <row r="101" spans="1:25" ht="15.75" customHeight="1">
       <c r="A101" s="5">
         <v>41</v>
       </c>
+      <c r="B101" s="14"/>
+      <c r="D101" s="145" t="s">
+        <v>111</v>
+      </c>
+      <c r="E101" s="149" t="str">
+        <f>IF(Q90="","",Q90)</f>
+        <v/>
+      </c>
+      <c r="M101" s="15"/>
       <c r="O101" s="109" t="str">
-        <f>IF(O60="","",O60)</f>
-        <v>Turbo</v>
+        <f>IF(O58="","",O58)</f>
+        <v>Array</v>
       </c>
       <c r="P101" s="89"/>
       <c r="Q101" s="89"/>
@@ -5287,42 +5364,120 @@
         <v/>
       </c>
       <c r="U101" s="95" t="str">
-        <f>IF(S101="","",S101*($O$92/$O$93)^2)</f>
+        <f>IF(S101="","",S101*($O$94/$O$95)^2)</f>
         <v/>
       </c>
       <c r="V101" s="95" t="str">
-        <f>IF(U101="","",U101/R60)</f>
+        <f>IF(U101="","",U101/R58)</f>
         <v/>
       </c>
       <c r="Y101" s="76"/>
     </row>
-    <row r="102" spans="1:25" ht="15.75" customHeight="1" thickBot="1">
+    <row r="102" spans="1:25" ht="15.75" customHeight="1">
       <c r="A102" s="5">
         <v>42</v>
       </c>
-      <c r="O102" s="80"/>
-      <c r="P102" s="81"/>
-      <c r="Q102" s="81"/>
-      <c r="R102" s="81"/>
-      <c r="S102" s="81"/>
-      <c r="T102" s="81"/>
-      <c r="U102" s="81"/>
-      <c r="V102" s="81"/>
-      <c r="W102" s="81"/>
-      <c r="X102" s="81"/>
-      <c r="Y102" s="82"/>
+      <c r="B102" s="14"/>
+      <c r="D102" s="145" t="s">
+        <v>109</v>
+      </c>
+      <c r="E102" s="150" t="str">
+        <f>IF(T90="","",T90)</f>
+        <v/>
+      </c>
+      <c r="M102" s="15"/>
+      <c r="O102" s="109" t="str">
+        <f>IF(O59="","",O59)</f>
+        <v>Fast Array</v>
+      </c>
+      <c r="P102" s="89"/>
+      <c r="Q102" s="89"/>
+      <c r="R102" s="89"/>
+      <c r="S102" s="110" t="str">
+        <f>IF(P102="","",AVERAGE(P102:R102))</f>
+        <v/>
+      </c>
+      <c r="T102" s="110" t="str">
+        <f>IF(P102="","",STDEV(P102:R102))</f>
+        <v/>
+      </c>
+      <c r="U102" s="95" t="str">
+        <f>IF(S102="","",S102*($O$94/$O$95)^2)</f>
+        <v/>
+      </c>
+      <c r="V102" s="95" t="str">
+        <f>IF(U102="","",U102/R59)</f>
+        <v/>
+      </c>
+      <c r="Y102" s="76"/>
     </row>
     <row r="103" spans="1:25" ht="15.75" customHeight="1">
       <c r="A103" s="5">
         <v>43</v>
       </c>
-    </row>
-    <row r="104" spans="1:25" ht="15.75" customHeight="1">
+      <c r="B103" s="14"/>
+      <c r="D103" s="145" t="s">
+        <v>110</v>
+      </c>
+      <c r="E103" s="150" t="str">
+        <f>IF(W90="","",W90)</f>
+        <v/>
+      </c>
+      <c r="M103" s="15"/>
+      <c r="O103" s="109" t="str">
+        <f>IF(O60="","",O60)</f>
+        <v>Turbo</v>
+      </c>
+      <c r="P103" s="89"/>
+      <c r="Q103" s="89"/>
+      <c r="R103" s="89"/>
+      <c r="S103" s="110" t="str">
+        <f>IF(P103="","",AVERAGE(P103:R103))</f>
+        <v/>
+      </c>
+      <c r="T103" s="110" t="str">
+        <f>IF(P103="","",STDEV(P103:R103))</f>
+        <v/>
+      </c>
+      <c r="U103" s="95" t="str">
+        <f>IF(S103="","",S103*($O$94/$O$95)^2)</f>
+        <v/>
+      </c>
+      <c r="V103" s="95" t="str">
+        <f>IF(U103="","",U103/R60)</f>
+        <v/>
+      </c>
+      <c r="Y103" s="76"/>
+    </row>
+    <row r="104" spans="1:25" ht="15.75" customHeight="1" thickBot="1">
       <c r="A104" s="5">
         <v>44</v>
       </c>
-    </row>
-    <row r="105" spans="1:25" ht="15.75" customHeight="1">
+      <c r="B104" s="24"/>
+      <c r="C104" s="25"/>
+      <c r="D104" s="25"/>
+      <c r="E104" s="25"/>
+      <c r="F104" s="25"/>
+      <c r="G104" s="25"/>
+      <c r="H104" s="25"/>
+      <c r="I104" s="25"/>
+      <c r="J104" s="25"/>
+      <c r="K104" s="25"/>
+      <c r="L104" s="25"/>
+      <c r="M104" s="26"/>
+      <c r="O104" s="80"/>
+      <c r="P104" s="81"/>
+      <c r="Q104" s="81"/>
+      <c r="R104" s="81"/>
+      <c r="S104" s="81"/>
+      <c r="T104" s="81"/>
+      <c r="U104" s="81"/>
+      <c r="V104" s="81"/>
+      <c r="W104" s="81"/>
+      <c r="X104" s="81"/>
+      <c r="Y104" s="82"/>
+    </row>
+    <row r="105" spans="1:25" ht="15.75" customHeight="1" thickTop="1">
       <c r="A105" s="5">
         <v>45</v>
       </c>
@@ -5459,7 +5614,7 @@
       <c r="C119" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="D119" s="136" t="str">
+      <c r="D119" s="122" t="str">
         <f>IF($P$7="","",$P$7)</f>
         <v/>
       </c>
@@ -5507,48 +5662,48 @@
     </row>
   </sheetData>
   <mergeCells count="39">
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="K77:L77"/>
+    <mergeCell ref="I77:I78"/>
+    <mergeCell ref="J77:J78"/>
+    <mergeCell ref="R84:T84"/>
+    <mergeCell ref="S55:T55"/>
+    <mergeCell ref="R66:T66"/>
+    <mergeCell ref="R72:T72"/>
+    <mergeCell ref="R78:T78"/>
+    <mergeCell ref="U94:V94"/>
+    <mergeCell ref="U95:V95"/>
+    <mergeCell ref="K27:L27"/>
+    <mergeCell ref="F28:G28"/>
+    <mergeCell ref="F29:G29"/>
+    <mergeCell ref="F30:G30"/>
+    <mergeCell ref="L34:M34"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="K10:L10"/>
     <mergeCell ref="F11:G11"/>
     <mergeCell ref="K11:L11"/>
     <mergeCell ref="F12:G12"/>
     <mergeCell ref="K12:L12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="K27:L27"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="F29:G29"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="L34:M34"/>
-    <mergeCell ref="U96:V96"/>
-    <mergeCell ref="S55:T55"/>
-    <mergeCell ref="R66:T66"/>
-    <mergeCell ref="R72:T72"/>
-    <mergeCell ref="R78:T78"/>
-    <mergeCell ref="P97:R97"/>
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="K77:L77"/>
-    <mergeCell ref="I77:I78"/>
-    <mergeCell ref="J77:J78"/>
-    <mergeCell ref="R84:T84"/>
   </mergeCells>
   <conditionalFormatting sqref="L35:L39 L42:L43 L46:L49">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Fix cell formula for equipment calibration dates
</commit_message>
<xml_diff>
--- a/MUSCBoneDensity.xlsx
+++ b/MUSCBoneDensity.xlsx
@@ -977,7 +977,7 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="152">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1245,86 +1245,80 @@
     </xf>
     <xf numFmtId="169" fontId="4" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="169" fontId="4" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="169" fontId="4" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="10" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="10" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="10" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1701,7 +1695,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD125"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K100" sqref="K100"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -2023,19 +2019,19 @@
       <c r="E10" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="125" t="str">
+      <c r="F10" s="139" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="125"/>
+      <c r="G10" s="139"/>
       <c r="J10" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="125" t="str">
+      <c r="K10" s="139" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="125"/>
+      <c r="L10" s="139"/>
       <c r="M10" s="15"/>
       <c r="O10" s="55"/>
       <c r="P10" s="13"/>
@@ -2079,19 +2075,19 @@
       <c r="E11" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="126" t="str">
+      <c r="F11" s="142" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="126"/>
+      <c r="G11" s="142"/>
       <c r="J11" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="126" t="str">
+      <c r="K11" s="142" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="126"/>
+      <c r="L11" s="142"/>
       <c r="M11" s="15"/>
       <c r="O11" s="55"/>
       <c r="P11" s="13"/>
@@ -2135,19 +2131,19 @@
       <c r="E12" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="126" t="str">
+      <c r="F12" s="142" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="126"/>
+      <c r="G12" s="142"/>
       <c r="J12" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="127" t="str">
+      <c r="K12" s="144" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="127"/>
+      <c r="L12" s="144"/>
       <c r="M12" s="15"/>
       <c r="O12" s="55"/>
       <c r="P12" s="13"/>
@@ -2191,14 +2187,14 @@
       <c r="E13" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="126" t="str">
+      <c r="F13" s="142" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="126"/>
+      <c r="G13" s="142"/>
       <c r="J13" s="52"/>
-      <c r="K13" s="128"/>
-      <c r="L13" s="128"/>
+      <c r="K13" s="143"/>
+      <c r="L13" s="143"/>
       <c r="M13" s="15"/>
       <c r="O13" s="55"/>
       <c r="P13" s="13"/>
@@ -2299,19 +2295,19 @@
       <c r="E16" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="125" t="str">
+      <c r="F16" s="139" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="125"/>
+      <c r="G16" s="139"/>
       <c r="J16" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="K16" s="129" t="str">
+      <c r="K16" s="141" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="129"/>
+      <c r="L16" s="141"/>
       <c r="M16" s="15"/>
       <c r="O16" s="55"/>
       <c r="P16" s="62" t="s">
@@ -2347,19 +2343,19 @@
       <c r="E17" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="125" t="str">
+      <c r="F17" s="139" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="125"/>
+      <c r="G17" s="139"/>
       <c r="J17" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="K17" s="125" t="str">
+      <c r="K17" s="139" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="125"/>
+      <c r="L17" s="139"/>
       <c r="M17" s="15"/>
       <c r="O17" s="55"/>
       <c r="P17" s="13"/>
@@ -2403,19 +2399,19 @@
       <c r="E18" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="125" t="str">
+      <c r="F18" s="139" t="str">
         <f>IF(R19="","",R19)</f>
         <v/>
       </c>
-      <c r="G18" s="125"/>
+      <c r="G18" s="139"/>
       <c r="J18" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="125" t="str">
+      <c r="K18" s="139" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="125"/>
+      <c r="L18" s="139"/>
       <c r="M18" s="15"/>
       <c r="O18" s="55"/>
       <c r="P18" s="13"/>
@@ -2504,19 +2500,19 @@
       <c r="E21" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="125" t="str">
+      <c r="F21" s="139" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="125"/>
+      <c r="G21" s="139"/>
       <c r="J21" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="K21" s="125" t="str">
+      <c r="K21" s="139" t="str">
         <f>IF(V22="","",V22)</f>
         <v/>
       </c>
-      <c r="L21" s="125"/>
+      <c r="L21" s="139"/>
       <c r="M21" s="15"/>
       <c r="O21" s="55"/>
       <c r="P21" s="62" t="s">
@@ -2554,19 +2550,19 @@
       <c r="E22" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="129" t="str">
+      <c r="F22" s="141" t="str">
         <f>IF(R23="","",R23)</f>
         <v/>
       </c>
-      <c r="G22" s="129"/>
+      <c r="G22" s="141"/>
       <c r="J22" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="K22" s="125" t="str">
+      <c r="K22" s="139" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="125"/>
+      <c r="L22" s="139"/>
       <c r="M22" s="15"/>
       <c r="O22" s="55"/>
       <c r="P22" s="13"/>
@@ -2613,11 +2609,11 @@
       <c r="J23" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="K23" s="125" t="str">
+      <c r="K23" s="139" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="125"/>
+      <c r="L23" s="139"/>
       <c r="M23" s="15"/>
       <c r="O23" s="55"/>
       <c r="P23" s="13"/>
@@ -2661,11 +2657,11 @@
       <c r="E24" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="125" t="str">
+      <c r="F24" s="139" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="125"/>
+      <c r="G24" s="139"/>
       <c r="M24" s="15"/>
       <c r="O24" s="55"/>
       <c r="P24" s="62" t="s">
@@ -2706,11 +2702,11 @@
       <c r="E25" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="125" t="str">
+      <c r="F25" s="139" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="125"/>
+      <c r="G25" s="139"/>
       <c r="J25" s="61" t="s">
         <v>39</v>
       </c>
@@ -2752,19 +2748,19 @@
       <c r="E26" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="125" t="str">
+      <c r="F26" s="139" t="str">
         <f>IF(R27="","",R27)</f>
         <v/>
       </c>
-      <c r="G26" s="125"/>
+      <c r="G26" s="139"/>
       <c r="J26" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="K26" s="125" t="str">
+      <c r="K26" s="139" t="str">
         <f>IF(V27="","",V27)</f>
         <v/>
       </c>
-      <c r="L26" s="125"/>
+      <c r="L26" s="139"/>
       <c r="M26" s="15"/>
       <c r="O26" s="55"/>
       <c r="P26" s="13"/>
@@ -2808,11 +2804,11 @@
       <c r="J27" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="K27" s="125" t="str">
+      <c r="K27" s="139" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="125"/>
+      <c r="L27" s="139"/>
       <c r="M27" s="15"/>
       <c r="O27" s="55"/>
       <c r="P27" s="13"/>
@@ -2849,11 +2845,11 @@
       <c r="E28" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="125" t="str">
+      <c r="F28" s="139" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="125"/>
+      <c r="G28" s="139"/>
       <c r="M28" s="15"/>
       <c r="O28" s="55"/>
       <c r="P28" s="62" t="s">
@@ -2894,11 +2890,11 @@
       <c r="E29" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="125" t="str">
+      <c r="F29" s="139" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="125"/>
+      <c r="G29" s="139"/>
       <c r="M29" s="15"/>
       <c r="O29" s="55"/>
       <c r="P29" s="13"/>
@@ -2937,11 +2933,11 @@
       <c r="E30" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F30" s="125" t="str">
+      <c r="F30" s="139" t="str">
         <f>IF(R31="","",R31)</f>
         <v/>
       </c>
-      <c r="G30" s="125"/>
+      <c r="G30" s="139"/>
       <c r="M30" s="15"/>
       <c r="O30" s="55"/>
       <c r="P30" s="13"/>
@@ -3085,10 +3081,10 @@
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
-      <c r="L34" s="130" t="s">
+      <c r="L34" s="140" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="130"/>
+      <c r="M34" s="140"/>
       <c r="O34" s="13"/>
       <c r="P34" s="13"/>
       <c r="Q34" s="13"/>
@@ -3612,10 +3608,10 @@
         <v>55</v>
       </c>
       <c r="O55" s="75"/>
-      <c r="S55" s="131" t="s">
+      <c r="S55" s="136" t="s">
         <v>68</v>
       </c>
-      <c r="T55" s="131"/>
+      <c r="T55" s="136"/>
       <c r="Y55" s="76"/>
     </row>
     <row r="56" spans="1:25" ht="15.75" customHeight="1">
@@ -3863,10 +3859,10 @@
         <v>4</v>
       </c>
       <c r="B64" s="14"/>
-      <c r="H64" s="132" t="s">
+      <c r="H64" s="128" t="s">
         <v>93</v>
       </c>
-      <c r="I64" s="133"/>
+      <c r="I64" s="129"/>
       <c r="K64" s="61" t="s">
         <v>67</v>
       </c>
@@ -3960,11 +3956,11 @@
       <c r="Q66" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="R66" s="131" t="s">
+      <c r="R66" s="136" t="s">
         <v>91</v>
       </c>
-      <c r="S66" s="131"/>
-      <c r="T66" s="131"/>
+      <c r="S66" s="136"/>
+      <c r="T66" s="136"/>
       <c r="U66" s="4" t="s">
         <v>91</v>
       </c>
@@ -4206,11 +4202,11 @@
       <c r="Q72" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="R72" s="131" t="s">
+      <c r="R72" s="136" t="s">
         <v>91</v>
       </c>
-      <c r="S72" s="131"/>
-      <c r="T72" s="131"/>
+      <c r="S72" s="136"/>
+      <c r="T72" s="136"/>
       <c r="U72" s="4" t="s">
         <v>91</v>
       </c>
@@ -4376,16 +4372,16 @@
       <c r="G77" s="97" t="s">
         <v>92</v>
       </c>
-      <c r="I77" s="136" t="s">
+      <c r="I77" s="132" t="s">
         <v>69</v>
       </c>
-      <c r="J77" s="138" t="s">
+      <c r="J77" s="134" t="s">
         <v>95</v>
       </c>
-      <c r="K77" s="134" t="s">
+      <c r="K77" s="130" t="s">
         <v>96</v>
       </c>
-      <c r="L77" s="135"/>
+      <c r="L77" s="131"/>
       <c r="M77" s="15"/>
       <c r="O77" s="75"/>
       <c r="Y77" s="76"/>
@@ -4411,8 +4407,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I78" s="137"/>
-      <c r="J78" s="139"/>
+      <c r="I78" s="133"/>
+      <c r="J78" s="135"/>
       <c r="K78" s="97" t="s">
         <v>97</v>
       </c>
@@ -4430,11 +4426,11 @@
       <c r="Q78" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="R78" s="131" t="s">
+      <c r="R78" s="136" t="s">
         <v>91</v>
       </c>
-      <c r="S78" s="131"/>
-      <c r="T78" s="131"/>
+      <c r="S78" s="136"/>
+      <c r="T78" s="136"/>
       <c r="U78" s="4" t="s">
         <v>91</v>
       </c>
@@ -4473,11 +4469,11 @@
         <v/>
       </c>
       <c r="K79" s="114" t="str">
-        <f>IF(U100="","",U100)</f>
+        <f t="shared" ref="K79:L82" si="7">IF(U100="","",U100)</f>
         <v/>
       </c>
       <c r="L79" s="114" t="str">
-        <f>IF(V100="","",V100)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="M79" s="15"/>
@@ -4533,11 +4529,11 @@
         <v/>
       </c>
       <c r="K80" s="114" t="str">
-        <f>IF(U101="","",U101)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L80" s="114" t="str">
-        <f>IF(V101="","",V101)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="M80" s="15"/>
@@ -4593,11 +4589,11 @@
         <v/>
       </c>
       <c r="K81" s="114" t="str">
-        <f>IF(U102="","",U102)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L81" s="114" t="str">
-        <f>IF(V102="","",V102)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="M81" s="15"/>
@@ -4637,11 +4633,11 @@
         <v/>
       </c>
       <c r="K82" s="114" t="str">
-        <f>IF(U103="","",U103)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="L82" s="114" t="str">
-        <f>IF(V103="","",V103)</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="M82" s="15"/>
@@ -4698,32 +4694,32 @@
       </c>
       <c r="B84" s="14"/>
       <c r="D84" s="97" t="str">
-        <f t="shared" ref="D84:E87" si="7">IF(P73="","",P73)</f>
+        <f t="shared" ref="D84:E87" si="8">IF(P73="","",P73)</f>
         <v>Tableside</v>
       </c>
       <c r="E84" s="118" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="F84" s="113" t="str">
-        <f t="shared" ref="F84:G87" si="8">IF(U73="","",U73)</f>
+        <f t="shared" ref="F84:G87" si="9">IF(U73="","",U73)</f>
         <v/>
       </c>
       <c r="G84" s="114" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="I84" s="145" t="s">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I84" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="J84" s="146" t="str">
+      <c r="J84" s="145" t="str">
         <f>IF(U94="","",U94)</f>
         <v>Piranha CB2-17090320</v>
       </c>
-      <c r="L84" s="151" t="s">
+      <c r="L84" s="147" t="s">
         <v>60</v>
       </c>
-      <c r="M84" s="153" t="str">
+      <c r="M84" s="148" t="str">
         <f>IF(X94="","",X94)</f>
         <v>R100B</v>
       </c>
@@ -4737,11 +4733,11 @@
       <c r="Q84" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="R84" s="131" t="s">
+      <c r="R84" s="136" t="s">
         <v>91</v>
       </c>
-      <c r="S84" s="131"/>
-      <c r="T84" s="131"/>
+      <c r="S84" s="136"/>
+      <c r="T84" s="136"/>
       <c r="U84" s="4" t="s">
         <v>91</v>
       </c>
@@ -4756,29 +4752,32 @@
       </c>
       <c r="B85" s="14"/>
       <c r="D85" s="97" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Operator</v>
       </c>
       <c r="E85" s="118" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="F85" s="113" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G85" s="114" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="I85" s="145" t="s">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I85" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="J85" s="147"/>
-      <c r="L85" s="151" t="s">
+      <c r="J85" s="146" t="str">
+        <f>IF(U96="","",U96)</f>
+        <v/>
+      </c>
+      <c r="L85" s="147" t="s">
         <v>109</v>
       </c>
-      <c r="M85" s="152" t="str">
+      <c r="M85" s="149" t="str">
         <f>IF(X96="","",X96)</f>
         <v/>
       </c>
@@ -4810,32 +4809,32 @@
       </c>
       <c r="B86" s="14"/>
       <c r="D86" s="97" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>Door</v>
       </c>
       <c r="E86" s="118" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="F86" s="113" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G86" s="114" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="I86" s="145" t="s">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+      <c r="I86" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="J86" s="148" t="str">
-        <f>IF(U96="","",U96)</f>
-        <v/>
-      </c>
-      <c r="L86" s="151" t="s">
+      <c r="J86" s="146" t="str">
+        <f>IF(U97="","",U97)</f>
+        <v/>
+      </c>
+      <c r="L86" s="147" t="s">
         <v>110</v>
       </c>
-      <c r="M86" s="152" t="str">
+      <c r="M86" s="149" t="str">
         <f>IF(X97="","",X97)</f>
         <v/>
       </c>
@@ -4867,19 +4866,19 @@
       </c>
       <c r="B87" s="14"/>
       <c r="D87" s="97" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="E87" s="118" t="str">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="F87" s="113" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="G87" s="114" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v/>
       </c>
       <c r="M87" s="15"/>
@@ -4964,19 +4963,19 @@
       </c>
       <c r="B90" s="14"/>
       <c r="D90" s="97" t="str">
-        <f t="shared" ref="D90:E93" si="9">IF(P79="","",P79)</f>
+        <f t="shared" ref="D90:E93" si="10">IF(P79="","",P79)</f>
         <v>Tableside</v>
       </c>
       <c r="E90" s="118" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F90" s="113" t="str">
-        <f t="shared" ref="F90:G93" si="10">IF(U79="","",U79)</f>
+        <f t="shared" ref="F90:G93" si="11">IF(U79="","",U79)</f>
         <v/>
       </c>
       <c r="G90" s="114" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="M90" s="15"/>
@@ -4984,15 +4983,15 @@
       <c r="P90" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="Q90" s="140"/>
+      <c r="Q90" s="125"/>
       <c r="S90" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="T90" s="142"/>
+      <c r="T90" s="127"/>
       <c r="V90" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="W90" s="142"/>
+      <c r="W90" s="127"/>
       <c r="Y90" s="76"/>
     </row>
     <row r="91" spans="1:25" ht="15.75" customHeight="1" thickBot="1">
@@ -5001,19 +5000,19 @@
       </c>
       <c r="B91" s="14"/>
       <c r="D91" s="97" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Operator</v>
       </c>
       <c r="E91" s="118" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F91" s="113" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="G91" s="114" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="M91" s="15"/>
@@ -5035,19 +5034,19 @@
       </c>
       <c r="B92" s="14"/>
       <c r="D92" s="97" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>Door</v>
       </c>
       <c r="E92" s="118" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F92" s="113" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="G92" s="114" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="M92" s="15"/>
@@ -5069,19 +5068,19 @@
       </c>
       <c r="B93" s="14"/>
       <c r="D93" s="97" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="E93" s="118" t="str">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v/>
       </c>
       <c r="F93" s="113" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="G93" s="114" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v/>
       </c>
       <c r="M93" s="15"/>
@@ -5105,15 +5104,15 @@
       <c r="T94" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="U94" s="143" t="str">
+      <c r="U94" s="137" t="str">
         <f>IF(U95&lt;&gt;"",U95,IF(AB42="","",AB42))</f>
         <v>Piranha CB2-17090320</v>
       </c>
-      <c r="V94" s="143"/>
+      <c r="V94" s="137"/>
       <c r="W94" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="X94" s="141" t="str">
+      <c r="X94" s="126" t="str">
         <f>IF(X95&lt;&gt;"",X95,IF(AB43="","",AB43))</f>
         <v>R100B</v>
       </c>
@@ -5147,11 +5146,11 @@
       <c r="P95" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="U95" s="144" t="s">
+      <c r="U95" s="138" t="s">
         <v>103</v>
       </c>
-      <c r="V95" s="144"/>
-      <c r="X95" s="140" t="s">
+      <c r="V95" s="138"/>
+      <c r="X95" s="125" t="s">
         <v>112</v>
       </c>
       <c r="Y95" s="76"/>
@@ -5162,19 +5161,19 @@
       </c>
       <c r="B96" s="14"/>
       <c r="D96" s="97" t="str">
-        <f t="shared" ref="D96:E99" si="11">IF(P85="","",P85)</f>
+        <f t="shared" ref="D96:E99" si="12">IF(P85="","",P85)</f>
         <v>Tableside</v>
       </c>
       <c r="E96" s="118" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="F96" s="113" t="str">
-        <f t="shared" ref="F96:G99" si="12">IF(U85="","",U85)</f>
+        <f t="shared" ref="F96:G99" si="13">IF(U85="","",U85)</f>
         <v/>
       </c>
       <c r="G96" s="114" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="M96" s="15"/>
@@ -5182,11 +5181,11 @@
       <c r="T96" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="U96" s="142"/>
+      <c r="U96" s="127"/>
       <c r="W96" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="X96" s="142"/>
+      <c r="X96" s="127"/>
       <c r="Y96" s="76"/>
     </row>
     <row r="97" spans="1:25" ht="15.75" customHeight="1">
@@ -5195,19 +5194,19 @@
       </c>
       <c r="B97" s="14"/>
       <c r="D97" s="97" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Operator</v>
       </c>
       <c r="E97" s="118" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="F97" s="113" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="G97" s="114" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="M97" s="15"/>
@@ -5217,11 +5216,11 @@
       <c r="T97" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="U97" s="142"/>
+      <c r="U97" s="127"/>
       <c r="W97" s="22" t="s">
         <v>110</v>
       </c>
-      <c r="X97" s="142"/>
+      <c r="X97" s="127"/>
       <c r="Y97" s="76"/>
     </row>
     <row r="98" spans="1:25" ht="15.75" customHeight="1">
@@ -5230,19 +5229,19 @@
       </c>
       <c r="B98" s="14"/>
       <c r="D98" s="97" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>Door</v>
       </c>
       <c r="E98" s="118" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="F98" s="113" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="G98" s="114" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="M98" s="15"/>
@@ -5266,19 +5265,19 @@
       </c>
       <c r="B99" s="14"/>
       <c r="D99" s="97" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="E99" s="118" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v/>
       </c>
       <c r="F99" s="113" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="G99" s="114" t="str">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v/>
       </c>
       <c r="M99" s="15"/>
@@ -5340,10 +5339,10 @@
         <v>41</v>
       </c>
       <c r="B101" s="14"/>
-      <c r="D101" s="145" t="s">
+      <c r="D101" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="E101" s="149" t="str">
+      <c r="E101" s="150" t="str">
         <f>IF(Q90="","",Q90)</f>
         <v/>
       </c>
@@ -5378,10 +5377,10 @@
         <v>42</v>
       </c>
       <c r="B102" s="14"/>
-      <c r="D102" s="145" t="s">
+      <c r="D102" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="E102" s="150" t="str">
+      <c r="E102" s="151" t="str">
         <f>IF(T90="","",T90)</f>
         <v/>
       </c>
@@ -5416,10 +5415,10 @@
         <v>43</v>
       </c>
       <c r="B103" s="14"/>
-      <c r="D103" s="145" t="s">
+      <c r="D103" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="E103" s="150" t="str">
+      <c r="E103" s="151" t="str">
         <f>IF(W90="","",W90)</f>
         <v/>
       </c>
@@ -5662,45 +5661,45 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="H64:I64"/>
-    <mergeCell ref="K77:L77"/>
-    <mergeCell ref="I77:I78"/>
-    <mergeCell ref="J77:J78"/>
-    <mergeCell ref="R84:T84"/>
-    <mergeCell ref="S55:T55"/>
-    <mergeCell ref="R66:T66"/>
-    <mergeCell ref="R72:T72"/>
-    <mergeCell ref="R78:T78"/>
-    <mergeCell ref="U94:V94"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="K26:L26"/>
     <mergeCell ref="U95:V95"/>
     <mergeCell ref="K27:L27"/>
     <mergeCell ref="F28:G28"/>
     <mergeCell ref="F29:G29"/>
     <mergeCell ref="F30:G30"/>
     <mergeCell ref="L34:M34"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="S55:T55"/>
+    <mergeCell ref="R66:T66"/>
+    <mergeCell ref="R72:T72"/>
+    <mergeCell ref="R78:T78"/>
+    <mergeCell ref="U94:V94"/>
+    <mergeCell ref="H64:I64"/>
+    <mergeCell ref="K77:L77"/>
+    <mergeCell ref="I77:I78"/>
+    <mergeCell ref="J77:J78"/>
+    <mergeCell ref="R84:T84"/>
   </mergeCells>
   <conditionalFormatting sqref="L35:L39 L42:L43 L46:L49">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">

</xml_diff>

<commit_message>
Add checks for new installs
</commit_message>
<xml_diff>
--- a/MUSCBoneDensity.xlsx
+++ b/MUSCBoneDensity.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugenem\Documents\GitHub\EquipTestingSpreadsheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maheug\Documents\GitHub\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A477F6DE-8019-4151-B70A-841B4DD085C6}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,8 +18,13 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$M$120</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="114">
   <si>
     <t>Print Area</t>
   </si>
@@ -366,12 +372,15 @@
   </si>
   <si>
     <t>R100B</t>
+  </si>
+  <si>
+    <t>Unit installed as shown on shielding plan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="dd\-mmm\-yy"/>
@@ -478,7 +487,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="44">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -961,6 +970,19 @@
       </right>
       <top/>
       <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -977,7 +999,7 @@
       <alignment horizontal="center" textRotation="90"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="154">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1248,6 +1270,54 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="169" fontId="4" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1272,63 +1342,31 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="42" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Heading" xfId="3"/>
-    <cellStyle name="Heading1" xfId="4"/>
+    <cellStyle name="Heading" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Heading1" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Result" xfId="1"/>
-    <cellStyle name="Result2" xfId="2"/>
+    <cellStyle name="Result" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Result2" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1692,22 +1730,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K100" sqref="K100"/>
+    <sheetView tabSelected="1" topLeftCell="C32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P52" sqref="P52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="2.5703125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="2.5703125" style="2" customWidth="1"/>
-    <col min="3" max="13" width="11.5703125" style="2"/>
-    <col min="14" max="14" width="2.5703125" style="3" customWidth="1"/>
-    <col min="15" max="28" width="11.5703125" style="3"/>
-    <col min="29" max="29" width="11.5703125" style="4"/>
-    <col min="30" max="30" width="11.5703125" style="3"/>
+    <col min="1" max="1" width="2.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="2.5546875" style="2" customWidth="1"/>
+    <col min="3" max="13" width="11.5546875" style="2"/>
+    <col min="14" max="14" width="2.5546875" style="3" customWidth="1"/>
+    <col min="15" max="28" width="11.5546875" style="3"/>
+    <col min="29" max="29" width="11.5546875" style="4"/>
+    <col min="30" max="30" width="11.5546875" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" ht="15.75" customHeight="1">
@@ -2019,19 +2057,19 @@
       <c r="E10" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="139" t="str">
+      <c r="F10" s="135" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="139"/>
+      <c r="G10" s="135"/>
       <c r="J10" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="139" t="str">
+      <c r="K10" s="135" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="139"/>
+      <c r="L10" s="135"/>
       <c r="M10" s="15"/>
       <c r="O10" s="55"/>
       <c r="P10" s="13"/>
@@ -2075,19 +2113,19 @@
       <c r="E11" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="142" t="str">
+      <c r="F11" s="136" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="142"/>
+      <c r="G11" s="136"/>
       <c r="J11" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="142" t="str">
+      <c r="K11" s="136" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="142"/>
+      <c r="L11" s="136"/>
       <c r="M11" s="15"/>
       <c r="O11" s="55"/>
       <c r="P11" s="13"/>
@@ -2131,19 +2169,19 @@
       <c r="E12" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="142" t="str">
+      <c r="F12" s="136" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="142"/>
+      <c r="G12" s="136"/>
       <c r="J12" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="144" t="str">
+      <c r="K12" s="137" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="144"/>
+      <c r="L12" s="137"/>
       <c r="M12" s="15"/>
       <c r="O12" s="55"/>
       <c r="P12" s="13"/>
@@ -2187,14 +2225,14 @@
       <c r="E13" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="142" t="str">
+      <c r="F13" s="136" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="142"/>
+      <c r="G13" s="136"/>
       <c r="J13" s="52"/>
-      <c r="K13" s="143"/>
-      <c r="L13" s="143"/>
+      <c r="K13" s="138"/>
+      <c r="L13" s="138"/>
       <c r="M13" s="15"/>
       <c r="O13" s="55"/>
       <c r="P13" s="13"/>
@@ -2295,19 +2333,19 @@
       <c r="E16" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="139" t="str">
+      <c r="F16" s="135" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="139"/>
+      <c r="G16" s="135"/>
       <c r="J16" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="K16" s="141" t="str">
+      <c r="K16" s="139" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="141"/>
+      <c r="L16" s="139"/>
       <c r="M16" s="15"/>
       <c r="O16" s="55"/>
       <c r="P16" s="62" t="s">
@@ -2343,19 +2381,19 @@
       <c r="E17" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="139" t="str">
+      <c r="F17" s="135" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="139"/>
+      <c r="G17" s="135"/>
       <c r="J17" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="K17" s="139" t="str">
+      <c r="K17" s="135" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="139"/>
+      <c r="L17" s="135"/>
       <c r="M17" s="15"/>
       <c r="O17" s="55"/>
       <c r="P17" s="13"/>
@@ -2399,19 +2437,19 @@
       <c r="E18" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="139" t="str">
+      <c r="F18" s="135" t="str">
         <f>IF(R19="","",R19)</f>
         <v/>
       </c>
-      <c r="G18" s="139"/>
+      <c r="G18" s="135"/>
       <c r="J18" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="139" t="str">
+      <c r="K18" s="135" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="139"/>
+      <c r="L18" s="135"/>
       <c r="M18" s="15"/>
       <c r="O18" s="55"/>
       <c r="P18" s="13"/>
@@ -2500,19 +2538,19 @@
       <c r="E21" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="139" t="str">
+      <c r="F21" s="135" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="139"/>
+      <c r="G21" s="135"/>
       <c r="J21" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="K21" s="139" t="str">
+      <c r="K21" s="135" t="str">
         <f>IF(V22="","",V22)</f>
         <v/>
       </c>
-      <c r="L21" s="139"/>
+      <c r="L21" s="135"/>
       <c r="M21" s="15"/>
       <c r="O21" s="55"/>
       <c r="P21" s="62" t="s">
@@ -2550,19 +2588,19 @@
       <c r="E22" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="141" t="str">
+      <c r="F22" s="139" t="str">
         <f>IF(R23="","",R23)</f>
         <v/>
       </c>
-      <c r="G22" s="141"/>
+      <c r="G22" s="139"/>
       <c r="J22" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="K22" s="139" t="str">
+      <c r="K22" s="135" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="139"/>
+      <c r="L22" s="135"/>
       <c r="M22" s="15"/>
       <c r="O22" s="55"/>
       <c r="P22" s="13"/>
@@ -2609,11 +2647,11 @@
       <c r="J23" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="K23" s="139" t="str">
+      <c r="K23" s="135" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="139"/>
+      <c r="L23" s="135"/>
       <c r="M23" s="15"/>
       <c r="O23" s="55"/>
       <c r="P23" s="13"/>
@@ -2657,11 +2695,11 @@
       <c r="E24" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="139" t="str">
+      <c r="F24" s="135" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="139"/>
+      <c r="G24" s="135"/>
       <c r="M24" s="15"/>
       <c r="O24" s="55"/>
       <c r="P24" s="62" t="s">
@@ -2702,11 +2740,11 @@
       <c r="E25" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="139" t="str">
+      <c r="F25" s="135" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="139"/>
+      <c r="G25" s="135"/>
       <c r="J25" s="61" t="s">
         <v>39</v>
       </c>
@@ -2748,19 +2786,19 @@
       <c r="E26" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="139" t="str">
+      <c r="F26" s="135" t="str">
         <f>IF(R27="","",R27)</f>
         <v/>
       </c>
-      <c r="G26" s="139"/>
+      <c r="G26" s="135"/>
       <c r="J26" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="K26" s="139" t="str">
+      <c r="K26" s="135" t="str">
         <f>IF(V27="","",V27)</f>
         <v/>
       </c>
-      <c r="L26" s="139"/>
+      <c r="L26" s="135"/>
       <c r="M26" s="15"/>
       <c r="O26" s="55"/>
       <c r="P26" s="13"/>
@@ -2804,11 +2842,11 @@
       <c r="J27" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="K27" s="139" t="str">
+      <c r="K27" s="135" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="139"/>
+      <c r="L27" s="135"/>
       <c r="M27" s="15"/>
       <c r="O27" s="55"/>
       <c r="P27" s="13"/>
@@ -2845,11 +2883,11 @@
       <c r="E28" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="139" t="str">
+      <c r="F28" s="135" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="139"/>
+      <c r="G28" s="135"/>
       <c r="M28" s="15"/>
       <c r="O28" s="55"/>
       <c r="P28" s="62" t="s">
@@ -2890,11 +2928,11 @@
       <c r="E29" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="139" t="str">
+      <c r="F29" s="135" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="139"/>
+      <c r="G29" s="135"/>
       <c r="M29" s="15"/>
       <c r="O29" s="55"/>
       <c r="P29" s="13"/>
@@ -2933,11 +2971,11 @@
       <c r="E30" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F30" s="139" t="str">
+      <c r="F30" s="135" t="str">
         <f>IF(R31="","",R31)</f>
         <v/>
       </c>
-      <c r="G30" s="139"/>
+      <c r="G30" s="135"/>
       <c r="M30" s="15"/>
       <c r="O30" s="55"/>
       <c r="P30" s="13"/>
@@ -3081,10 +3119,10 @@
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
-      <c r="L34" s="140" t="s">
+      <c r="L34" s="141" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="140"/>
+      <c r="M34" s="141"/>
       <c r="O34" s="13"/>
       <c r="P34" s="13"/>
       <c r="Q34" s="13"/>
@@ -3529,21 +3567,26 @@
       </c>
       <c r="Y49" s="76"/>
     </row>
-    <row r="50" spans="1:25" ht="15.75" customHeight="1">
+    <row r="50" spans="1:25" ht="15.75" customHeight="1" thickBot="1">
       <c r="A50" s="5">
         <v>50</v>
       </c>
       <c r="B50" s="24"/>
       <c r="C50" s="25"/>
       <c r="D50" s="25"/>
-      <c r="E50" s="25"/>
+      <c r="E50" s="25" t="s">
+        <v>113</v>
+      </c>
       <c r="F50" s="25"/>
       <c r="G50" s="25"/>
       <c r="H50" s="25"/>
       <c r="I50" s="25"/>
       <c r="J50" s="25"/>
       <c r="K50" s="25"/>
-      <c r="L50" s="25"/>
+      <c r="L50" s="153" t="str">
+        <f>IF(O52="","TBD",IF(O52=1,"YES",IF(O52=3,"NA","")))</f>
+        <v>NA</v>
+      </c>
       <c r="M50" s="26"/>
       <c r="O50" s="77"/>
       <c r="P50" s="23" t="s">
@@ -3551,7 +3594,7 @@
       </c>
       <c r="Y50" s="76"/>
     </row>
-    <row r="51" spans="1:25" ht="15.75" customHeight="1">
+    <row r="51" spans="1:25" ht="15.75" customHeight="1" thickTop="1">
       <c r="A51" s="5">
         <v>51</v>
       </c>
@@ -3561,13 +3604,17 @@
       </c>
       <c r="Y51" s="76"/>
     </row>
-    <row r="52" spans="1:25" ht="15.75" customHeight="1">
+    <row r="52" spans="1:25" ht="15.75" customHeight="1" thickBot="1">
       <c r="A52" s="5">
         <v>52</v>
       </c>
       <c r="H52" s="37"/>
-      <c r="O52" s="80"/>
-      <c r="P52" s="81"/>
+      <c r="O52" s="152">
+        <v>3</v>
+      </c>
+      <c r="P52" s="81" t="s">
+        <v>113</v>
+      </c>
       <c r="Q52" s="81"/>
       <c r="R52" s="81"/>
       <c r="S52" s="81"/>
@@ -3578,7 +3625,7 @@
       <c r="X52" s="81"/>
       <c r="Y52" s="82"/>
     </row>
-    <row r="53" spans="1:25" ht="15.75" customHeight="1">
+    <row r="53" spans="1:25" ht="15.75" customHeight="1" thickBot="1">
       <c r="A53" s="5">
         <v>53</v>
       </c>
@@ -3608,10 +3655,10 @@
         <v>55</v>
       </c>
       <c r="O55" s="75"/>
-      <c r="S55" s="136" t="s">
+      <c r="S55" s="142" t="s">
         <v>68</v>
       </c>
-      <c r="T55" s="136"/>
+      <c r="T55" s="142"/>
       <c r="Y55" s="76"/>
     </row>
     <row r="56" spans="1:25" ht="15.75" customHeight="1">
@@ -3859,10 +3906,10 @@
         <v>4</v>
       </c>
       <c r="B64" s="14"/>
-      <c r="H64" s="128" t="s">
+      <c r="H64" s="144" t="s">
         <v>93</v>
       </c>
-      <c r="I64" s="129"/>
+      <c r="I64" s="145"/>
       <c r="K64" s="61" t="s">
         <v>67</v>
       </c>
@@ -3956,11 +4003,11 @@
       <c r="Q66" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="R66" s="136" t="s">
+      <c r="R66" s="142" t="s">
         <v>91</v>
       </c>
-      <c r="S66" s="136"/>
-      <c r="T66" s="136"/>
+      <c r="S66" s="142"/>
+      <c r="T66" s="142"/>
       <c r="U66" s="4" t="s">
         <v>91</v>
       </c>
@@ -4202,11 +4249,11 @@
       <c r="Q72" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="R72" s="136" t="s">
+      <c r="R72" s="142" t="s">
         <v>91</v>
       </c>
-      <c r="S72" s="136"/>
-      <c r="T72" s="136"/>
+      <c r="S72" s="142"/>
+      <c r="T72" s="142"/>
       <c r="U72" s="4" t="s">
         <v>91</v>
       </c>
@@ -4372,16 +4419,16 @@
       <c r="G77" s="97" t="s">
         <v>92</v>
       </c>
-      <c r="I77" s="132" t="s">
+      <c r="I77" s="148" t="s">
         <v>69</v>
       </c>
-      <c r="J77" s="134" t="s">
+      <c r="J77" s="150" t="s">
         <v>95</v>
       </c>
-      <c r="K77" s="130" t="s">
+      <c r="K77" s="146" t="s">
         <v>96</v>
       </c>
-      <c r="L77" s="131"/>
+      <c r="L77" s="147"/>
       <c r="M77" s="15"/>
       <c r="O77" s="75"/>
       <c r="Y77" s="76"/>
@@ -4407,8 +4454,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I78" s="133"/>
-      <c r="J78" s="135"/>
+      <c r="I78" s="149"/>
+      <c r="J78" s="151"/>
       <c r="K78" s="97" t="s">
         <v>97</v>
       </c>
@@ -4426,11 +4473,11 @@
       <c r="Q78" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="R78" s="136" t="s">
+      <c r="R78" s="142" t="s">
         <v>91</v>
       </c>
-      <c r="S78" s="136"/>
-      <c r="T78" s="136"/>
+      <c r="S78" s="142"/>
+      <c r="T78" s="142"/>
       <c r="U78" s="4" t="s">
         <v>91</v>
       </c>
@@ -4712,14 +4759,14 @@
       <c r="I84" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="J84" s="145" t="str">
+      <c r="J84" s="128" t="str">
         <f>IF(U94="","",U94)</f>
         <v>Piranha CB2-17090320</v>
       </c>
-      <c r="L84" s="147" t="s">
+      <c r="L84" s="130" t="s">
         <v>60</v>
       </c>
-      <c r="M84" s="148" t="str">
+      <c r="M84" s="131" t="str">
         <f>IF(X94="","",X94)</f>
         <v>R100B</v>
       </c>
@@ -4733,11 +4780,11 @@
       <c r="Q84" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="R84" s="136" t="s">
+      <c r="R84" s="142" t="s">
         <v>91</v>
       </c>
-      <c r="S84" s="136"/>
-      <c r="T84" s="136"/>
+      <c r="S84" s="142"/>
+      <c r="T84" s="142"/>
       <c r="U84" s="4" t="s">
         <v>91</v>
       </c>
@@ -4770,14 +4817,14 @@
       <c r="I85" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="J85" s="146" t="str">
+      <c r="J85" s="129" t="str">
         <f>IF(U96="","",U96)</f>
         <v/>
       </c>
-      <c r="L85" s="147" t="s">
+      <c r="L85" s="130" t="s">
         <v>109</v>
       </c>
-      <c r="M85" s="149" t="str">
+      <c r="M85" s="132" t="str">
         <f>IF(X96="","",X96)</f>
         <v/>
       </c>
@@ -4827,14 +4874,14 @@
       <c r="I86" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="J86" s="146" t="str">
+      <c r="J86" s="129" t="str">
         <f>IF(U97="","",U97)</f>
         <v/>
       </c>
-      <c r="L86" s="147" t="s">
+      <c r="L86" s="130" t="s">
         <v>110</v>
       </c>
-      <c r="M86" s="149" t="str">
+      <c r="M86" s="132" t="str">
         <f>IF(X97="","",X97)</f>
         <v/>
       </c>
@@ -5104,11 +5151,11 @@
       <c r="T94" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="U94" s="137" t="str">
+      <c r="U94" s="143" t="str">
         <f>IF(U95&lt;&gt;"",U95,IF(AB42="","",AB42))</f>
         <v>Piranha CB2-17090320</v>
       </c>
-      <c r="V94" s="137"/>
+      <c r="V94" s="143"/>
       <c r="W94" s="22" t="s">
         <v>60</v>
       </c>
@@ -5146,10 +5193,10 @@
       <c r="P95" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="U95" s="138" t="s">
+      <c r="U95" s="140" t="s">
         <v>103</v>
       </c>
-      <c r="V95" s="138"/>
+      <c r="V95" s="140"/>
       <c r="X95" s="125" t="s">
         <v>112</v>
       </c>
@@ -5342,7 +5389,7 @@
       <c r="D101" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="E101" s="150" t="str">
+      <c r="E101" s="133" t="str">
         <f>IF(Q90="","",Q90)</f>
         <v/>
       </c>
@@ -5380,7 +5427,7 @@
       <c r="D102" s="52" t="s">
         <v>109</v>
       </c>
-      <c r="E102" s="151" t="str">
+      <c r="E102" s="134" t="str">
         <f>IF(T90="","",T90)</f>
         <v/>
       </c>
@@ -5418,7 +5465,7 @@
       <c r="D103" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="E103" s="151" t="str">
+      <c r="E103" s="134" t="str">
         <f>IF(W90="","",W90)</f>
         <v/>
       </c>
@@ -5661,29 +5708,6 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="K26:L26"/>
     <mergeCell ref="U95:V95"/>
     <mergeCell ref="K27:L27"/>
     <mergeCell ref="F28:G28"/>
@@ -5700,15 +5724,43 @@
     <mergeCell ref="I77:I78"/>
     <mergeCell ref="J77:J78"/>
     <mergeCell ref="R84:T84"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
   </mergeCells>
   <conditionalFormatting sqref="L35:L39 L42:L43 L46:L49">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M35:M39 M42:M43 M46:M49">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"NO"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L50">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"NO"</formula>
+      <formula>"TBD"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.5" right="0.5" top="0.59861111111111098" bottom="0.73750000000000004" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Turn off Track Changes
Track Changes was causing problems with Ocean2014 sending data to the spreadsheets
</commit_message>
<xml_diff>
--- a/MUSCBoneDensity.xlsx
+++ b/MUSCBoneDensity.xlsx
@@ -1300,12 +1300,24 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1338,18 +1350,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1469,24 +1469,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{365164B5-DA74-46DD-9CB4-F2E36D7F5BF5}">
-  <header guid="{365164B5-DA74-46DD-9CB4-F2E36D7F5BF5}" dateTime="2020-06-03T09:43:54" maxSheetId="2" userName="Eugene Mah" r:id="rId1">
-    <sheetIdMap count="1">
-      <sheetId val="1"/>
-    </sheetIdMap>
-  </header>
-</headers>
-</file>
-
-<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
-<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
-</file>
-
-<file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
-<users xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" count="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2076,19 +2058,19 @@
       <c r="E10" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="138" t="str">
+      <c r="F10" s="137" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="138"/>
+      <c r="G10" s="137"/>
       <c r="J10" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="138" t="str">
+      <c r="K10" s="137" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="138"/>
+      <c r="L10" s="137"/>
       <c r="M10" s="15"/>
       <c r="O10" s="55"/>
       <c r="P10" s="13"/>
@@ -2132,19 +2114,19 @@
       <c r="E11" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="151" t="str">
+      <c r="F11" s="138" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="151"/>
+      <c r="G11" s="138"/>
       <c r="J11" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="151" t="str">
+      <c r="K11" s="138" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="151"/>
+      <c r="L11" s="138"/>
       <c r="M11" s="15"/>
       <c r="O11" s="55"/>
       <c r="P11" s="13"/>
@@ -2188,19 +2170,19 @@
       <c r="E12" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="151" t="str">
+      <c r="F12" s="138" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="151"/>
+      <c r="G12" s="138"/>
       <c r="J12" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="153" t="str">
+      <c r="K12" s="139" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="153"/>
+      <c r="L12" s="139"/>
       <c r="M12" s="15"/>
       <c r="O12" s="55"/>
       <c r="P12" s="13"/>
@@ -2244,14 +2226,14 @@
       <c r="E13" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="151" t="str">
+      <c r="F13" s="138" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="151"/>
+      <c r="G13" s="138"/>
       <c r="J13" s="52"/>
-      <c r="K13" s="152"/>
-      <c r="L13" s="152"/>
+      <c r="K13" s="140"/>
+      <c r="L13" s="140"/>
       <c r="M13" s="15"/>
       <c r="O13" s="55"/>
       <c r="P13" s="13"/>
@@ -2352,19 +2334,19 @@
       <c r="E16" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="138" t="str">
+      <c r="F16" s="137" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="138"/>
+      <c r="G16" s="137"/>
       <c r="J16" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="K16" s="150" t="str">
+      <c r="K16" s="141" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="150"/>
+      <c r="L16" s="141"/>
       <c r="M16" s="15"/>
       <c r="O16" s="55"/>
       <c r="P16" s="62" t="s">
@@ -2400,19 +2382,19 @@
       <c r="E17" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="138" t="str">
+      <c r="F17" s="137" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="138"/>
+      <c r="G17" s="137"/>
       <c r="J17" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="K17" s="138" t="str">
+      <c r="K17" s="137" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="138"/>
+      <c r="L17" s="137"/>
       <c r="M17" s="15"/>
       <c r="O17" s="55"/>
       <c r="P17" s="13"/>
@@ -2456,19 +2438,19 @@
       <c r="E18" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="138" t="str">
+      <c r="F18" s="137" t="str">
         <f>IF(R19="","",R19)</f>
         <v/>
       </c>
-      <c r="G18" s="138"/>
+      <c r="G18" s="137"/>
       <c r="J18" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="138" t="str">
+      <c r="K18" s="137" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="138"/>
+      <c r="L18" s="137"/>
       <c r="M18" s="15"/>
       <c r="O18" s="55"/>
       <c r="P18" s="13"/>
@@ -2557,19 +2539,19 @@
       <c r="E21" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="138" t="str">
+      <c r="F21" s="137" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="138"/>
+      <c r="G21" s="137"/>
       <c r="J21" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="K21" s="138" t="str">
+      <c r="K21" s="137" t="str">
         <f>IF(V22="","",V22)</f>
         <v/>
       </c>
-      <c r="L21" s="138"/>
+      <c r="L21" s="137"/>
       <c r="M21" s="15"/>
       <c r="O21" s="55"/>
       <c r="P21" s="62" t="s">
@@ -2607,19 +2589,19 @@
       <c r="E22" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="150" t="str">
+      <c r="F22" s="141" t="str">
         <f>IF(R23="","",R23)</f>
         <v/>
       </c>
-      <c r="G22" s="150"/>
+      <c r="G22" s="141"/>
       <c r="J22" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="K22" s="138" t="str">
+      <c r="K22" s="137" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="138"/>
+      <c r="L22" s="137"/>
       <c r="M22" s="15"/>
       <c r="O22" s="55"/>
       <c r="P22" s="13"/>
@@ -2666,11 +2648,11 @@
       <c r="J23" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="K23" s="138" t="str">
+      <c r="K23" s="137" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="138"/>
+      <c r="L23" s="137"/>
       <c r="M23" s="15"/>
       <c r="O23" s="55"/>
       <c r="P23" s="13"/>
@@ -2714,11 +2696,11 @@
       <c r="E24" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="138" t="str">
+      <c r="F24" s="137" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="138"/>
+      <c r="G24" s="137"/>
       <c r="M24" s="15"/>
       <c r="O24" s="55"/>
       <c r="P24" s="62" t="s">
@@ -2759,11 +2741,11 @@
       <c r="E25" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="138" t="str">
+      <c r="F25" s="137" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="138"/>
+      <c r="G25" s="137"/>
       <c r="J25" s="61" t="s">
         <v>39</v>
       </c>
@@ -2805,19 +2787,19 @@
       <c r="E26" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="138" t="str">
+      <c r="F26" s="137" t="str">
         <f>IF(R27="","",R27)</f>
         <v/>
       </c>
-      <c r="G26" s="138"/>
+      <c r="G26" s="137"/>
       <c r="J26" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="K26" s="138" t="str">
+      <c r="K26" s="137" t="str">
         <f>IF(V27="","",V27)</f>
         <v/>
       </c>
-      <c r="L26" s="138"/>
+      <c r="L26" s="137"/>
       <c r="M26" s="15"/>
       <c r="O26" s="55"/>
       <c r="P26" s="13"/>
@@ -2861,11 +2843,11 @@
       <c r="J27" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="K27" s="138" t="str">
+      <c r="K27" s="137" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="138"/>
+      <c r="L27" s="137"/>
       <c r="M27" s="15"/>
       <c r="O27" s="55"/>
       <c r="P27" s="13"/>
@@ -2902,11 +2884,11 @@
       <c r="E28" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="138" t="str">
+      <c r="F28" s="137" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="138"/>
+      <c r="G28" s="137"/>
       <c r="M28" s="15"/>
       <c r="O28" s="55"/>
       <c r="P28" s="62" t="s">
@@ -2947,11 +2929,11 @@
       <c r="E29" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="138" t="str">
+      <c r="F29" s="137" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="138"/>
+      <c r="G29" s="137"/>
       <c r="M29" s="15"/>
       <c r="O29" s="55"/>
       <c r="P29" s="13"/>
@@ -2990,11 +2972,11 @@
       <c r="E30" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F30" s="138" t="str">
+      <c r="F30" s="137" t="str">
         <f>IF(R31="","",R31)</f>
         <v/>
       </c>
-      <c r="G30" s="138"/>
+      <c r="G30" s="137"/>
       <c r="M30" s="15"/>
       <c r="O30" s="55"/>
       <c r="P30" s="13"/>
@@ -3138,10 +3120,10 @@
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
-      <c r="L34" s="139" t="s">
+      <c r="L34" s="143" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="139"/>
+      <c r="M34" s="143"/>
       <c r="O34" s="13"/>
       <c r="P34" s="13"/>
       <c r="Q34" s="13"/>
@@ -3674,10 +3656,10 @@
         <v>55</v>
       </c>
       <c r="O55" s="75"/>
-      <c r="S55" s="140" t="s">
+      <c r="S55" s="144" t="s">
         <v>68</v>
       </c>
-      <c r="T55" s="140"/>
+      <c r="T55" s="144"/>
       <c r="Y55" s="76"/>
     </row>
     <row r="56" spans="1:25" ht="15.75" customHeight="1">
@@ -3925,10 +3907,10 @@
         <v>4</v>
       </c>
       <c r="B64" s="14"/>
-      <c r="H64" s="142" t="s">
+      <c r="H64" s="146" t="s">
         <v>93</v>
       </c>
-      <c r="I64" s="143"/>
+      <c r="I64" s="147"/>
       <c r="K64" s="61" t="s">
         <v>67</v>
       </c>
@@ -4022,11 +4004,11 @@
       <c r="Q66" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="R66" s="140" t="s">
+      <c r="R66" s="144" t="s">
         <v>91</v>
       </c>
-      <c r="S66" s="140"/>
-      <c r="T66" s="140"/>
+      <c r="S66" s="144"/>
+      <c r="T66" s="144"/>
       <c r="U66" s="4" t="s">
         <v>91</v>
       </c>
@@ -4268,11 +4250,11 @@
       <c r="Q72" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="R72" s="140" t="s">
+      <c r="R72" s="144" t="s">
         <v>91</v>
       </c>
-      <c r="S72" s="140"/>
-      <c r="T72" s="140"/>
+      <c r="S72" s="144"/>
+      <c r="T72" s="144"/>
       <c r="U72" s="4" t="s">
         <v>91</v>
       </c>
@@ -4438,16 +4420,16 @@
       <c r="G77" s="97" t="s">
         <v>92</v>
       </c>
-      <c r="I77" s="146" t="s">
+      <c r="I77" s="150" t="s">
         <v>69</v>
       </c>
-      <c r="J77" s="148" t="s">
+      <c r="J77" s="152" t="s">
         <v>95</v>
       </c>
-      <c r="K77" s="144" t="s">
+      <c r="K77" s="148" t="s">
         <v>96</v>
       </c>
-      <c r="L77" s="145"/>
+      <c r="L77" s="149"/>
       <c r="M77" s="15"/>
       <c r="O77" s="75"/>
       <c r="Y77" s="76"/>
@@ -4473,8 +4455,8 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I78" s="147"/>
-      <c r="J78" s="149"/>
+      <c r="I78" s="151"/>
+      <c r="J78" s="153"/>
       <c r="K78" s="97" t="s">
         <v>97</v>
       </c>
@@ -4492,11 +4474,11 @@
       <c r="Q78" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="R78" s="140" t="s">
+      <c r="R78" s="144" t="s">
         <v>91</v>
       </c>
-      <c r="S78" s="140"/>
-      <c r="T78" s="140"/>
+      <c r="S78" s="144"/>
+      <c r="T78" s="144"/>
       <c r="U78" s="4" t="s">
         <v>91</v>
       </c>
@@ -4799,11 +4781,11 @@
       <c r="Q84" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="R84" s="140" t="s">
+      <c r="R84" s="144" t="s">
         <v>91</v>
       </c>
-      <c r="S84" s="140"/>
-      <c r="T84" s="140"/>
+      <c r="S84" s="144"/>
+      <c r="T84" s="144"/>
       <c r="U84" s="4" t="s">
         <v>91</v>
       </c>
@@ -5170,11 +5152,11 @@
       <c r="T94" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="U94" s="141" t="str">
+      <c r="U94" s="145" t="str">
         <f>IF(U95&lt;&gt;"",U95,IF(AB42="","",AB42))</f>
         <v>Piranha CB2-17090320</v>
       </c>
-      <c r="V94" s="141"/>
+      <c r="V94" s="145"/>
       <c r="W94" s="22" t="s">
         <v>60</v>
       </c>
@@ -5212,10 +5194,10 @@
       <c r="P95" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="U95" s="137" t="s">
+      <c r="U95" s="142" t="s">
         <v>103</v>
       </c>
-      <c r="V95" s="137"/>
+      <c r="V95" s="142"/>
       <c r="X95" s="125" t="s">
         <v>112</v>
       </c>
@@ -5736,29 +5718,6 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="39">
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="K26:L26"/>
     <mergeCell ref="U95:V95"/>
     <mergeCell ref="K27:L27"/>
     <mergeCell ref="F28:G28"/>
@@ -5775,6 +5734,29 @@
     <mergeCell ref="I77:I78"/>
     <mergeCell ref="J77:J78"/>
     <mergeCell ref="R84:T84"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="K26:L26"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
   </mergeCells>
   <conditionalFormatting sqref="L35:L39 L42:L43 L46:L49">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">

</xml_diff>

<commit_message>
Update references to DHEC rule numbers
References to DHEC rule numbers updated to the most recent DHEC Title B revision (26-May-2023)
</commit_message>
<xml_diff>
--- a/MUSCBoneDensity.xlsx
+++ b/MUSCBoneDensity.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eugenem\Documents\GitHub\EquipTestingSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{126C78CB-AFCE-4430-891F-B40C1178F619}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +21,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$B$1:$M$120</definedName>
     <definedName name="Z_FCFD580C_7BEB_4F5F_B2A6_4586EBD853CD_.wvu.PrintArea" localSheetId="0" hidden="1">Sheet1!$B$1:$M$120</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <customWorkbookViews>
     <customWorkbookView name="Eugene Mah - Personal View" guid="{FCFD580C-7BEB-4F5F-B2A6-4586EBD853CD}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="784" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
@@ -28,6 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -38,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="116">
   <si>
     <t>Print Area</t>
   </si>
@@ -190,9 +194,6 @@
     <t>Enter 1 for YES, 2 for NO, 3 for NA</t>
   </si>
   <si>
-    <t>DHEC RHB 10.2.1</t>
-  </si>
-  <si>
     <t>DHEC RHB 4.3.1</t>
   </si>
   <si>
@@ -383,12 +384,18 @@
   </si>
   <si>
     <t>Page1,Page2</t>
+  </si>
+  <si>
+    <t>DHEC RHB 11.2.3</t>
+  </si>
+  <si>
+    <t>DHEC RHB 4.10.3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="6">
     <numFmt numFmtId="164" formatCode="[$$-409]#,##0.00;[Red]\-[$$-409]#,##0.00"/>
     <numFmt numFmtId="165" formatCode="dd\-mmm\-yy"/>
@@ -1305,64 +1312,64 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Heading" xfId="3"/>
-    <cellStyle name="Heading1" xfId="4"/>
+    <cellStyle name="Heading" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Heading1" xfId="4" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Result" xfId="1"/>
-    <cellStyle name="Result2" xfId="2"/>
+    <cellStyle name="Result" xfId="1" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Result2" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="3">
     <dxf>
@@ -1738,7 +1745,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AD125"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
@@ -1771,7 +1778,7 @@
       <c r="L1" s="7"/>
       <c r="M1" s="8"/>
       <c r="O1" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P1" s="10"/>
       <c r="Q1" s="10"/>
@@ -1812,7 +1819,7 @@
       <c r="X2" s="13"/>
       <c r="Y2" s="18"/>
       <c r="AA2" s="19" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AB2" s="13"/>
       <c r="AD2" s="13"/>
@@ -1868,7 +1875,7 @@
         <v>3</v>
       </c>
       <c r="AB4" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="AD4" s="13"/>
     </row>
@@ -2067,19 +2074,19 @@
       <c r="E10" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="137" t="str">
+      <c r="F10" s="138" t="str">
         <f>IF(R10="","",R10)</f>
         <v/>
       </c>
-      <c r="G10" s="137"/>
+      <c r="G10" s="138"/>
       <c r="J10" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="K10" s="137" t="str">
+      <c r="K10" s="138" t="str">
         <f>IF(V10="","",V10)</f>
         <v/>
       </c>
-      <c r="L10" s="137"/>
+      <c r="L10" s="138"/>
       <c r="M10" s="15"/>
       <c r="O10" s="55"/>
       <c r="P10" s="13"/>
@@ -2123,19 +2130,19 @@
       <c r="E11" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="138" t="str">
+      <c r="F11" s="151" t="str">
         <f>IF(R11="","",R11)</f>
         <v/>
       </c>
-      <c r="G11" s="138"/>
+      <c r="G11" s="151"/>
       <c r="J11" s="52" t="s">
         <v>20</v>
       </c>
-      <c r="K11" s="138" t="str">
+      <c r="K11" s="151" t="str">
         <f>IF(V11="","",V11)</f>
         <v/>
       </c>
-      <c r="L11" s="138"/>
+      <c r="L11" s="151"/>
       <c r="M11" s="15"/>
       <c r="O11" s="55"/>
       <c r="P11" s="13"/>
@@ -2179,19 +2186,19 @@
       <c r="E12" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="138" t="str">
+      <c r="F12" s="151" t="str">
         <f>IF(R12="","",R12)</f>
         <v/>
       </c>
-      <c r="G12" s="138"/>
+      <c r="G12" s="151"/>
       <c r="J12" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="K12" s="139" t="str">
+      <c r="K12" s="153" t="str">
         <f>IF(V12="","",V12)</f>
         <v/>
       </c>
-      <c r="L12" s="139"/>
+      <c r="L12" s="153"/>
       <c r="M12" s="15"/>
       <c r="O12" s="55"/>
       <c r="P12" s="13"/>
@@ -2235,14 +2242,14 @@
       <c r="E13" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="138" t="str">
+      <c r="F13" s="151" t="str">
         <f>IF(R13="","",R13)</f>
         <v/>
       </c>
-      <c r="G13" s="138"/>
+      <c r="G13" s="151"/>
       <c r="J13" s="52"/>
-      <c r="K13" s="140"/>
-      <c r="L13" s="140"/>
+      <c r="K13" s="152"/>
+      <c r="L13" s="152"/>
       <c r="M13" s="15"/>
       <c r="O13" s="55"/>
       <c r="P13" s="13"/>
@@ -2343,19 +2350,19 @@
       <c r="E16" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F16" s="137" t="str">
+      <c r="F16" s="138" t="str">
         <f>IF(R17="","",R17)</f>
         <v/>
       </c>
-      <c r="G16" s="137"/>
+      <c r="G16" s="138"/>
       <c r="J16" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="K16" s="141" t="str">
+      <c r="K16" s="150" t="str">
         <f>IF(V17="","",V17)</f>
         <v/>
       </c>
-      <c r="L16" s="141"/>
+      <c r="L16" s="150"/>
       <c r="M16" s="15"/>
       <c r="O16" s="55"/>
       <c r="P16" s="62" t="s">
@@ -2391,19 +2398,19 @@
       <c r="E17" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="F17" s="137" t="str">
+      <c r="F17" s="138" t="str">
         <f>IF(R18="","",R18)</f>
         <v/>
       </c>
-      <c r="G17" s="137"/>
+      <c r="G17" s="138"/>
       <c r="J17" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="K17" s="137" t="str">
+      <c r="K17" s="138" t="str">
         <f>IF(V18="","",V18)</f>
         <v/>
       </c>
-      <c r="L17" s="137"/>
+      <c r="L17" s="138"/>
       <c r="M17" s="15"/>
       <c r="O17" s="55"/>
       <c r="P17" s="13"/>
@@ -2447,19 +2454,19 @@
       <c r="E18" s="52" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="137" t="str">
+      <c r="F18" s="138" t="str">
         <f>IF(R19="","",R19)</f>
         <v/>
       </c>
-      <c r="G18" s="137"/>
+      <c r="G18" s="138"/>
       <c r="J18" s="52" t="s">
         <v>31</v>
       </c>
-      <c r="K18" s="137" t="str">
+      <c r="K18" s="138" t="str">
         <f>IF(V19="","",V19)</f>
         <v/>
       </c>
-      <c r="L18" s="137"/>
+      <c r="L18" s="138"/>
       <c r="M18" s="15"/>
       <c r="O18" s="55"/>
       <c r="P18" s="13"/>
@@ -2548,19 +2555,19 @@
       <c r="E21" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="137" t="str">
+      <c r="F21" s="138" t="str">
         <f>IF(R22="","",R22)</f>
         <v/>
       </c>
-      <c r="G21" s="137"/>
+      <c r="G21" s="138"/>
       <c r="J21" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="K21" s="137" t="str">
+      <c r="K21" s="138" t="str">
         <f>IF(V22="","",V22)</f>
         <v/>
       </c>
-      <c r="L21" s="137"/>
+      <c r="L21" s="138"/>
       <c r="M21" s="15"/>
       <c r="O21" s="55"/>
       <c r="P21" s="62" t="s">
@@ -2598,19 +2605,19 @@
       <c r="E22" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="F22" s="141" t="str">
+      <c r="F22" s="150" t="str">
         <f>IF(R23="","",R23)</f>
         <v/>
       </c>
-      <c r="G22" s="141"/>
+      <c r="G22" s="150"/>
       <c r="J22" s="52" t="s">
         <v>36</v>
       </c>
-      <c r="K22" s="137" t="str">
+      <c r="K22" s="138" t="str">
         <f>IF(V23="","",V23)</f>
         <v/>
       </c>
-      <c r="L22" s="137"/>
+      <c r="L22" s="138"/>
       <c r="M22" s="15"/>
       <c r="O22" s="55"/>
       <c r="P22" s="13"/>
@@ -2657,11 +2664,11 @@
       <c r="J23" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="K23" s="137" t="str">
+      <c r="K23" s="138" t="str">
         <f>IF(V24="","",V24)</f>
         <v/>
       </c>
-      <c r="L23" s="137"/>
+      <c r="L23" s="138"/>
       <c r="M23" s="15"/>
       <c r="O23" s="55"/>
       <c r="P23" s="13"/>
@@ -2705,11 +2712,11 @@
       <c r="E24" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F24" s="137" t="str">
+      <c r="F24" s="138" t="str">
         <f>IF(R25="","",R25)</f>
         <v/>
       </c>
-      <c r="G24" s="137"/>
+      <c r="G24" s="138"/>
       <c r="M24" s="15"/>
       <c r="O24" s="55"/>
       <c r="P24" s="62" t="s">
@@ -2750,11 +2757,11 @@
       <c r="E25" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="137" t="str">
+      <c r="F25" s="138" t="str">
         <f>IF(R26="","",R26)</f>
         <v/>
       </c>
-      <c r="G25" s="137"/>
+      <c r="G25" s="138"/>
       <c r="J25" s="61" t="s">
         <v>39</v>
       </c>
@@ -2796,19 +2803,19 @@
       <c r="E26" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="137" t="str">
+      <c r="F26" s="138" t="str">
         <f>IF(R27="","",R27)</f>
         <v/>
       </c>
-      <c r="G26" s="137"/>
+      <c r="G26" s="138"/>
       <c r="J26" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="K26" s="137" t="str">
+      <c r="K26" s="138" t="str">
         <f>IF(V27="","",V27)</f>
         <v/>
       </c>
-      <c r="L26" s="137"/>
+      <c r="L26" s="138"/>
       <c r="M26" s="15"/>
       <c r="O26" s="55"/>
       <c r="P26" s="13"/>
@@ -2852,11 +2859,11 @@
       <c r="J27" s="52" t="s">
         <v>42</v>
       </c>
-      <c r="K27" s="137" t="str">
+      <c r="K27" s="138" t="str">
         <f>IF(V28="","",V28)</f>
         <v/>
       </c>
-      <c r="L27" s="137"/>
+      <c r="L27" s="138"/>
       <c r="M27" s="15"/>
       <c r="O27" s="55"/>
       <c r="P27" s="13"/>
@@ -2893,11 +2900,11 @@
       <c r="E28" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="137" t="str">
+      <c r="F28" s="138" t="str">
         <f>IF(R29="","",R29)</f>
         <v/>
       </c>
-      <c r="G28" s="137"/>
+      <c r="G28" s="138"/>
       <c r="M28" s="15"/>
       <c r="O28" s="55"/>
       <c r="P28" s="62" t="s">
@@ -2938,11 +2945,11 @@
       <c r="E29" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="F29" s="137" t="str">
+      <c r="F29" s="138" t="str">
         <f>IF(R30="","",R30)</f>
         <v/>
       </c>
-      <c r="G29" s="137"/>
+      <c r="G29" s="138"/>
       <c r="M29" s="15"/>
       <c r="O29" s="55"/>
       <c r="P29" s="13"/>
@@ -2981,11 +2988,11 @@
       <c r="E30" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F30" s="137" t="str">
+      <c r="F30" s="138" t="str">
         <f>IF(R31="","",R31)</f>
         <v/>
       </c>
-      <c r="G30" s="137"/>
+      <c r="G30" s="138"/>
       <c r="M30" s="15"/>
       <c r="O30" s="55"/>
       <c r="P30" s="13"/>
@@ -3129,10 +3136,10 @@
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
-      <c r="L34" s="143" t="s">
+      <c r="L34" s="139" t="s">
         <v>46</v>
       </c>
-      <c r="M34" s="143"/>
+      <c r="M34" s="139"/>
       <c r="O34" s="13"/>
       <c r="P34" s="13"/>
       <c r="Q34" s="13"/>
@@ -3210,10 +3217,10 @@
       </c>
       <c r="B36" s="14"/>
       <c r="C36" s="71" t="s">
-        <v>50</v>
+        <v>114</v>
       </c>
       <c r="E36" s="72" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L36" s="73" t="str">
         <f>IF(O38="","TBD",IF(O38=1,"YES",IF(O38=3,"NA","")))</f>
@@ -3247,10 +3254,10 @@
       </c>
       <c r="B37" s="14"/>
       <c r="C37" s="71" t="s">
+        <v>50</v>
+      </c>
+      <c r="E37" s="72" t="s">
         <v>51</v>
-      </c>
-      <c r="E37" s="72" t="s">
-        <v>52</v>
       </c>
       <c r="L37" s="73" t="str">
         <f>IF(O39="","TBD",IF(O39=1,"YES",IF(O39=3,"NA","")))</f>
@@ -3285,7 +3292,7 @@
       <c r="B38" s="14"/>
       <c r="C38" s="71"/>
       <c r="E38" s="72" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L38" s="73" t="str">
         <f>IF(O40="","TBD",IF(O40=1,"YES",IF(O40=3,"NA","")))</f>
@@ -3297,7 +3304,7 @@
       </c>
       <c r="O38" s="77"/>
       <c r="P38" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="Y38" s="76"/>
       <c r="AA38" s="22" t="s">
@@ -3320,7 +3327,7 @@
       <c r="B39" s="14"/>
       <c r="C39" s="71"/>
       <c r="E39" s="72" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="L39" s="73" t="str">
         <f>IF(O41="","TBD",IF(O41=1,"YES",IF(O41=3,"NA","")))</f>
@@ -3332,7 +3339,7 @@
       </c>
       <c r="O39" s="77"/>
       <c r="P39" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Y39" s="76"/>
       <c r="AA39" s="22" t="s">
@@ -3359,7 +3366,7 @@
       <c r="M40" s="78"/>
       <c r="O40" s="77"/>
       <c r="P40" s="23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="Y40" s="76"/>
       <c r="AA40" s="22" t="s">
@@ -3382,13 +3389,13 @@
       <c r="B41" s="14"/>
       <c r="C41" s="71"/>
       <c r="F41" s="61" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="L41" s="21"/>
       <c r="M41" s="79"/>
       <c r="O41" s="77"/>
       <c r="P41" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Y41" s="76"/>
     </row>
@@ -3399,7 +3406,7 @@
       <c r="B42" s="14"/>
       <c r="C42" s="71"/>
       <c r="E42" s="72" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L42" s="73" t="str">
         <f>IF(O44="","TBD",IF(O44=1,"YES",IF(O44=3,"NA","")))</f>
@@ -3412,7 +3419,7 @@
       <c r="O42" s="75"/>
       <c r="Y42" s="76"/>
       <c r="AA42" s="22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AB42" s="49"/>
       <c r="AC42" s="35" t="str">
@@ -3429,8 +3436,11 @@
         <v>43</v>
       </c>
       <c r="B43" s="14"/>
+      <c r="C43" s="71" t="s">
+        <v>115</v>
+      </c>
       <c r="E43" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L43" s="73" t="str">
         <f>IF(O45="","TBD",IF(O45=1,"YES",IF(O45=3,"NA","")))</f>
@@ -3442,11 +3452,11 @@
       </c>
       <c r="O43" s="75"/>
       <c r="T43" s="39" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Y43" s="76"/>
       <c r="AA43" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB43" s="49"/>
       <c r="AC43" s="35" t="str">
@@ -3467,7 +3477,7 @@
       <c r="M44" s="79"/>
       <c r="O44" s="77"/>
       <c r="P44" s="23" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="Y44" s="76"/>
     </row>
@@ -3478,13 +3488,13 @@
       <c r="B45" s="14"/>
       <c r="C45" s="51"/>
       <c r="F45" s="61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L45" s="21"/>
       <c r="M45" s="79"/>
       <c r="O45" s="77"/>
       <c r="P45" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y45" s="76"/>
     </row>
@@ -3495,7 +3505,7 @@
       <c r="B46" s="14"/>
       <c r="C46" s="51"/>
       <c r="E46" s="72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="L46" s="73" t="str">
         <f>IF(O48="","TBD",IF(O48=1,"YES",IF(O48=3,"NA","")))</f>
@@ -3515,7 +3525,7 @@
       <c r="B47" s="14"/>
       <c r="C47" s="51"/>
       <c r="E47" s="72" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L47" s="73" t="str">
         <f>IF(O49="","TBD",IF(O49=1,"YES",IF(O49=3,"NA","")))</f>
@@ -3527,7 +3537,7 @@
       </c>
       <c r="O47" s="75"/>
       <c r="T47" s="39" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Y47" s="76"/>
     </row>
@@ -3538,7 +3548,7 @@
       <c r="B48" s="14"/>
       <c r="C48" s="51"/>
       <c r="E48" s="72" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L48" s="73" t="str">
         <f>IF(O50="","TBD",IF(O50=1,"YES",IF(O50=3,"NA","")))</f>
@@ -3550,7 +3560,7 @@
       </c>
       <c r="O48" s="77"/>
       <c r="P48" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Y48" s="76"/>
     </row>
@@ -3561,7 +3571,7 @@
       <c r="B49" s="14"/>
       <c r="C49" s="51"/>
       <c r="E49" s="72" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L49" s="73" t="str">
         <f>IF(O51="","TBD",IF(O51=1,"YES",IF(O51=3,"NA","")))</f>
@@ -3573,7 +3583,7 @@
       </c>
       <c r="O49" s="77"/>
       <c r="P49" s="23" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="Y49" s="76"/>
     </row>
@@ -3585,7 +3595,7 @@
       <c r="C50" s="25"/>
       <c r="D50" s="25"/>
       <c r="E50" s="25" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F50" s="25"/>
       <c r="G50" s="25"/>
@@ -3600,7 +3610,7 @@
       <c r="M50" s="26"/>
       <c r="O50" s="77"/>
       <c r="P50" s="23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Y50" s="76"/>
     </row>
@@ -3610,7 +3620,7 @@
       </c>
       <c r="O51" s="77"/>
       <c r="P51" s="23" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y51" s="76"/>
     </row>
@@ -3623,7 +3633,7 @@
         <v>3</v>
       </c>
       <c r="P52" s="81" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="Q52" s="81"/>
       <c r="R52" s="81"/>
@@ -3645,7 +3655,7 @@
         <v>54</v>
       </c>
       <c r="O54" s="83" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="P54" s="84"/>
       <c r="Q54" s="84"/>
@@ -3654,7 +3664,7 @@
       <c r="T54" s="84"/>
       <c r="U54" s="84"/>
       <c r="V54" s="85" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="W54" s="84"/>
       <c r="X54" s="84"/>
@@ -3665,10 +3675,10 @@
         <v>55</v>
       </c>
       <c r="O55" s="75"/>
-      <c r="S55" s="144" t="s">
-        <v>67</v>
-      </c>
-      <c r="T55" s="144"/>
+      <c r="S55" s="140" t="s">
+        <v>66</v>
+      </c>
+      <c r="T55" s="140"/>
       <c r="Y55" s="76"/>
     </row>
     <row r="56" spans="1:25" ht="15.75" customHeight="1">
@@ -3676,28 +3686,28 @@
         <v>56</v>
       </c>
       <c r="O56" s="87" t="s">
+        <v>67</v>
+      </c>
+      <c r="P56" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="P56" s="4" t="s">
+      <c r="Q56" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="Q56" s="4" t="s">
+      <c r="R56" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="R56" s="4" t="s">
+      <c r="S56" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="S56" s="4" t="s">
+      <c r="T56" s="4" t="s">
         <v>72</v>
-      </c>
-      <c r="T56" s="4" t="s">
-        <v>73</v>
       </c>
       <c r="V56" s="4" t="s">
         <v>14</v>
       </c>
       <c r="W56" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Y56" s="76"/>
     </row>
@@ -3706,10 +3716,10 @@
         <v>57</v>
       </c>
       <c r="O57" s="88" t="s">
+        <v>74</v>
+      </c>
+      <c r="P57" s="89" t="s">
         <v>75</v>
-      </c>
-      <c r="P57" s="89" t="s">
-        <v>76</v>
       </c>
       <c r="Q57" s="89">
         <v>2.5</v>
@@ -3726,7 +3736,7 @@
         <v>20.32</v>
       </c>
       <c r="V57" s="89" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="W57" s="89"/>
       <c r="Y57" s="76"/>
@@ -3736,10 +3746,10 @@
         <v>58</v>
       </c>
       <c r="O58" s="88" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="P58" s="89" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q58" s="89">
         <v>2.5</v>
@@ -3754,7 +3764,7 @@
         <v>20.32</v>
       </c>
       <c r="V58" s="89" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="W58" s="89"/>
       <c r="Y58" s="76"/>
@@ -3778,10 +3788,10 @@
         <v>Eugene Mah</v>
       </c>
       <c r="O59" s="88" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P59" s="89" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q59" s="89">
         <v>2.5</v>
@@ -3798,7 +3808,7 @@
         <v>20.32</v>
       </c>
       <c r="V59" s="89" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="W59" s="89"/>
       <c r="Y59" s="76"/>
@@ -3808,7 +3818,7 @@
         <v>60</v>
       </c>
       <c r="C60" s="52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D60" s="53" t="str">
         <f>IF($R$14="","",$R$14)</f>
@@ -3822,10 +3832,10 @@
         <v/>
       </c>
       <c r="O60" s="88" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="P60" s="89" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q60" s="89">
         <v>2.5</v>
@@ -3868,7 +3878,7 @@
         <v>Bone Mineral Density Compliance Inspection</v>
       </c>
       <c r="O62" s="90" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="Y62" s="76"/>
     </row>
@@ -3878,7 +3888,7 @@
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="42" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
@@ -3891,19 +3901,19 @@
       <c r="L63" s="7"/>
       <c r="M63" s="8"/>
       <c r="O63" s="91" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="P63" s="89">
         <v>82</v>
       </c>
       <c r="Q63" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="R63" s="89"/>
       <c r="S63" s="89"/>
       <c r="T63" s="89"/>
       <c r="V63" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="W63" s="92" t="str">
         <f>IF(R63="","",AVERAGE(R63:T63))</f>
@@ -3916,12 +3926,12 @@
         <v>4</v>
       </c>
       <c r="B64" s="14"/>
-      <c r="H64" s="146" t="s">
-        <v>92</v>
-      </c>
-      <c r="I64" s="147"/>
+      <c r="H64" s="142" t="s">
+        <v>91</v>
+      </c>
+      <c r="I64" s="143"/>
       <c r="K64" s="61" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M64" s="15"/>
       <c r="O64" s="75"/>
@@ -3933,35 +3943,35 @@
       </c>
       <c r="B65" s="14"/>
       <c r="D65" s="97" t="s">
+        <v>67</v>
+      </c>
+      <c r="E65" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="E65" s="97" t="s">
+      <c r="F65" s="97" t="s">
         <v>69</v>
       </c>
-      <c r="F65" s="97" t="s">
+      <c r="G65" s="97" t="s">
         <v>70</v>
       </c>
-      <c r="G65" s="97" t="s">
+      <c r="H65" s="98" t="s">
         <v>71</v>
       </c>
-      <c r="H65" s="98" t="s">
+      <c r="I65" s="99" t="s">
         <v>72</v>
-      </c>
-      <c r="I65" s="99" t="s">
-        <v>73</v>
       </c>
       <c r="K65" s="97" t="s">
         <v>14</v>
       </c>
       <c r="L65" s="111" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="M65" s="15"/>
       <c r="O65" s="90" t="s">
+        <v>86</v>
+      </c>
+      <c r="U65" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="U65" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="Y65" s="76"/>
     </row>
@@ -4011,18 +4021,18 @@
         <v>14</v>
       </c>
       <c r="Q66" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="R66" s="144" t="s">
+        <v>73</v>
+      </c>
+      <c r="R66" s="140" t="s">
+        <v>89</v>
+      </c>
+      <c r="S66" s="140"/>
+      <c r="T66" s="140"/>
+      <c r="U66" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="V66" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="S66" s="144"/>
-      <c r="T66" s="144"/>
-      <c r="U66" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="V66" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="Y66" s="76"/>
     </row>
@@ -4257,18 +4267,18 @@
         <v>14</v>
       </c>
       <c r="Q72" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="R72" s="144" t="s">
+        <v>73</v>
+      </c>
+      <c r="R72" s="140" t="s">
+        <v>89</v>
+      </c>
+      <c r="S72" s="140"/>
+      <c r="T72" s="140"/>
+      <c r="U72" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="V72" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="S72" s="144"/>
-      <c r="T72" s="144"/>
-      <c r="U72" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="V72" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="Y72" s="76"/>
     </row>
@@ -4344,7 +4354,7 @@
       </c>
       <c r="B75" s="115"/>
       <c r="C75" s="103" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D75" s="104"/>
       <c r="E75" s="104"/>
@@ -4352,7 +4362,7 @@
       <c r="G75" s="104"/>
       <c r="H75" s="104"/>
       <c r="I75" s="103" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="J75" s="104"/>
       <c r="K75" s="104"/>
@@ -4421,24 +4431,24 @@
         <v>14</v>
       </c>
       <c r="E77" s="112" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F77" s="97" t="s">
+        <v>89</v>
+      </c>
+      <c r="G77" s="97" t="s">
         <v>90</v>
       </c>
-      <c r="G77" s="97" t="s">
-        <v>91</v>
-      </c>
-      <c r="I77" s="150" t="s">
-        <v>68</v>
-      </c>
-      <c r="J77" s="152" t="s">
+      <c r="I77" s="146" t="s">
+        <v>67</v>
+      </c>
+      <c r="J77" s="148" t="s">
+        <v>93</v>
+      </c>
+      <c r="K77" s="144" t="s">
         <v>94</v>
       </c>
-      <c r="K77" s="148" t="s">
-        <v>95</v>
-      </c>
-      <c r="L77" s="149"/>
+      <c r="L77" s="145"/>
       <c r="M77" s="15"/>
       <c r="O77" s="75"/>
       <c r="Y77" s="76"/>
@@ -4464,13 +4474,13 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I78" s="151"/>
-      <c r="J78" s="153"/>
+      <c r="I78" s="147"/>
+      <c r="J78" s="149"/>
       <c r="K78" s="97" t="s">
+        <v>95</v>
+      </c>
+      <c r="L78" s="97" t="s">
         <v>96</v>
-      </c>
-      <c r="L78" s="97" t="s">
-        <v>97</v>
       </c>
       <c r="M78" s="15"/>
       <c r="O78" s="93" t="str">
@@ -4481,18 +4491,18 @@
         <v>14</v>
       </c>
       <c r="Q78" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="R78" s="144" t="s">
+        <v>73</v>
+      </c>
+      <c r="R78" s="140" t="s">
+        <v>89</v>
+      </c>
+      <c r="S78" s="140"/>
+      <c r="T78" s="140"/>
+      <c r="U78" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="V78" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="S78" s="144"/>
-      <c r="T78" s="144"/>
-      <c r="U78" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="V78" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="Y78" s="76"/>
     </row>
@@ -4733,13 +4743,13 @@
         <v>14</v>
       </c>
       <c r="E83" s="112" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F83" s="97" t="s">
+        <v>89</v>
+      </c>
+      <c r="G83" s="97" t="s">
         <v>90</v>
-      </c>
-      <c r="G83" s="97" t="s">
-        <v>91</v>
       </c>
       <c r="M83" s="15"/>
       <c r="O83" s="75"/>
@@ -4767,14 +4777,14 @@
         <v/>
       </c>
       <c r="I84" s="52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J84" s="128" t="str">
         <f>IF(U94="","",U94)</f>
         <v>Piranha CB2-17090320</v>
       </c>
       <c r="L84" s="130" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M84" s="131" t="str">
         <f>IF(X94="","",X94)</f>
@@ -4788,18 +4798,18 @@
         <v>14</v>
       </c>
       <c r="Q84" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="R84" s="144" t="s">
+        <v>73</v>
+      </c>
+      <c r="R84" s="140" t="s">
+        <v>89</v>
+      </c>
+      <c r="S84" s="140"/>
+      <c r="T84" s="140"/>
+      <c r="U84" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="V84" s="4" t="s">
         <v>90</v>
-      </c>
-      <c r="S84" s="144"/>
-      <c r="T84" s="144"/>
-      <c r="U84" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="V84" s="4" t="s">
-        <v>91</v>
       </c>
       <c r="Y84" s="76"/>
     </row>
@@ -4825,14 +4835,14 @@
         <v/>
       </c>
       <c r="I85" s="52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J85" s="129" t="str">
         <f>IF(U96="","",U96)</f>
         <v/>
       </c>
       <c r="L85" s="130" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M85" s="132" t="str">
         <f>IF(X96="","",X96)</f>
@@ -4882,14 +4892,14 @@
         <v/>
       </c>
       <c r="I86" s="52" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J86" s="129" t="str">
         <f>IF(U97="","",U97)</f>
         <v/>
       </c>
       <c r="L86" s="130" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M86" s="132" t="str">
         <f>IF(X97="","",X97)</f>
@@ -5002,13 +5012,13 @@
         <v>14</v>
       </c>
       <c r="E89" s="112" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F89" s="97" t="s">
+        <v>89</v>
+      </c>
+      <c r="G89" s="97" t="s">
         <v>90</v>
-      </c>
-      <c r="G89" s="97" t="s">
-        <v>91</v>
       </c>
       <c r="M89" s="15"/>
       <c r="O89" s="75"/>
@@ -5038,15 +5048,15 @@
       <c r="M90" s="15"/>
       <c r="O90" s="75"/>
       <c r="P90" s="22" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="Q90" s="125"/>
       <c r="S90" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T90" s="127"/>
       <c r="V90" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="W90" s="127"/>
       <c r="Y90" s="76"/>
@@ -5142,7 +5152,7 @@
       </c>
       <c r="M93" s="15"/>
       <c r="O93" s="90" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="Y93" s="76"/>
     </row>
@@ -5156,18 +5166,18 @@
         <v>107</v>
       </c>
       <c r="P94" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="T94" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="T94" s="22" t="s">
-        <v>100</v>
-      </c>
-      <c r="U94" s="145" t="str">
+      <c r="U94" s="141" t="str">
         <f>IF(U95&lt;&gt;"",U95,IF(AB42="","",AB42))</f>
         <v>Piranha CB2-17090320</v>
       </c>
-      <c r="V94" s="145"/>
+      <c r="V94" s="141"/>
       <c r="W94" s="22" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X94" s="126" t="str">
         <f>IF(X95&lt;&gt;"",X95,IF(AB43="","",AB43))</f>
@@ -5188,27 +5198,27 @@
         <v>14</v>
       </c>
       <c r="E95" s="112" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F95" s="97" t="s">
+        <v>89</v>
+      </c>
+      <c r="G95" s="97" t="s">
         <v>90</v>
-      </c>
-      <c r="G95" s="97" t="s">
-        <v>91</v>
       </c>
       <c r="M95" s="15"/>
       <c r="O95" s="77">
         <v>42.4</v>
       </c>
       <c r="P95" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="U95" s="137" t="s">
         <v>101</v>
       </c>
-      <c r="U95" s="142" t="s">
-        <v>102</v>
-      </c>
-      <c r="V95" s="142"/>
+      <c r="V95" s="137"/>
       <c r="X95" s="125" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="Y95" s="76"/>
     </row>
@@ -5236,11 +5246,11 @@
       <c r="M96" s="15"/>
       <c r="O96" s="75"/>
       <c r="T96" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="U96" s="127"/>
       <c r="W96" s="22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="X96" s="127"/>
       <c r="Y96" s="76"/>
@@ -5268,14 +5278,14 @@
       </c>
       <c r="M97" s="15"/>
       <c r="O97" s="90" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="T97" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="U97" s="127"/>
       <c r="W97" s="22" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="X97" s="127"/>
       <c r="Y97" s="76"/>
@@ -5307,11 +5317,11 @@
       <c r="Q98" s="106"/>
       <c r="R98" s="106"/>
       <c r="S98" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="T98" s="106"/>
       <c r="U98" s="119" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="V98" s="119"/>
       <c r="Y98" s="76"/>
@@ -5339,24 +5349,24 @@
       </c>
       <c r="M99" s="15"/>
       <c r="O99" s="108" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="P99" s="119" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="Q99" s="119"/>
       <c r="R99" s="119"/>
       <c r="S99" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="T99" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="U99" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="V99" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="T99" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="U99" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="V99" s="4" t="s">
-        <v>97</v>
       </c>
       <c r="Y99" s="76"/>
     </row>
@@ -5397,7 +5407,7 @@
       </c>
       <c r="B101" s="14"/>
       <c r="D101" s="52" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E101" s="133" t="str">
         <f>IF(Q90="","",Q90)</f>
@@ -5435,7 +5445,7 @@
       </c>
       <c r="B102" s="14"/>
       <c r="D102" s="52" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E102" s="134" t="str">
         <f>IF(T90="","",T90)</f>
@@ -5473,7 +5483,7 @@
       </c>
       <c r="B103" s="14"/>
       <c r="D103" s="52" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E103" s="134" t="str">
         <f>IF(W90="","",W90)</f>
@@ -5687,7 +5697,7 @@
         <v>60</v>
       </c>
       <c r="C120" s="52" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D120" s="54" t="str">
         <f>IF($R$14="","",$R$14)</f>
@@ -5727,6 +5737,29 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="39">
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="K10:L10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="K21:L21"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="K22:L22"/>
+    <mergeCell ref="K23:L23"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F26:G26"/>
+    <mergeCell ref="K26:L26"/>
     <mergeCell ref="U95:V95"/>
     <mergeCell ref="K27:L27"/>
     <mergeCell ref="F28:G28"/>
@@ -5743,29 +5776,6 @@
     <mergeCell ref="I77:I78"/>
     <mergeCell ref="J77:J78"/>
     <mergeCell ref="R84:T84"/>
-    <mergeCell ref="K23:L23"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="K26:L26"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="K21:L21"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="K22:L22"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="K13:L13"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="F17:G17"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="K10:L10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="K12:L12"/>
   </mergeCells>
   <conditionalFormatting sqref="L35:L39 L42:L43 L46:L49">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">

</xml_diff>